<commit_message>
all-best added max value
</commit_message>
<xml_diff>
--- a/MethodDemos/output/statistics/all-best-method-per-evaltype-publication-statistics.xlsx
+++ b/MethodDemos/output/statistics/all-best-method-per-evaltype-publication-statistics.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Cermine</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Summe</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -87,13 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1301,21 +1301,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B23" sqref="B23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="256" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="259" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>'[1]Tabelle 1'!A2</f>
         <v>Id</v>
@@ -1324,492 +1328,748 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>'[1]Tabelle 1'!A3</f>
         <v>Title</v>
       </c>
-      <c r="B2" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B3=MAX('[1]Tabelle 1'!B3:E3),"Cermine",IF('[1]Tabelle 1'!C3=MAX('[1]Tabelle 1'!B3:E3),"Grobid",IF('[1]Tabelle 1'!D3=MAX('[1]Tabelle 1'!B3:E3),"ParsCit",IF('[1]Tabelle 1'!E3=MAX('[1]Tabelle 1'!B3:E3),"PDFX","none"))))</f>
+      <c r="B2" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B3=C2,"Cermine",IF('[1]Tabelle 1'!C3=C2,"Grobid",IF('[1]Tabelle 1'!D3=C2,"ParsCit",IF('[1]Tabelle 1'!E3=C2,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="C2" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F3=MAX('[1]Tabelle 1'!F3:I3),"Cermine",IF('[1]Tabelle 1'!G3=MAX('[1]Tabelle 1'!F3:I3),"Grobid",IF('[1]Tabelle 1'!H3=MAX('[1]Tabelle 1'!F3:I3),"ParsCit",IF('[1]Tabelle 1'!I3=MAX('[1]Tabelle 1'!F3:I3),"PDFX","none"))))</f>
+      <c r="C2" s="3">
+        <f>MAX('[1]Tabelle 1'!B3:E3)</f>
+        <v>94.79</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F3=E2,"Cermine",IF('[1]Tabelle 1'!G3=E2,"Grobid",IF('[1]Tabelle 1'!H3=E2,"ParsCit",IF('[1]Tabelle 1'!I3=E2,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D2" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J3=MAX('[1]Tabelle 1'!J3:M3),"Cermine",IF('[1]Tabelle 1'!K3=MAX('[1]Tabelle 1'!J3:M3),"Grobid",IF('[1]Tabelle 1'!L3=MAX('[1]Tabelle 1'!J3:M3),"ParsCit",IF('[1]Tabelle 1'!M3=MAX('[1]Tabelle 1'!J3:M3),"PDFX","none"))))</f>
+      <c r="E2" s="3">
+        <f>MAX('[1]Tabelle 1'!F3:I3)</f>
+        <v>91</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J3=G2,"Cermine",IF('[1]Tabelle 1'!K3=G2,"Grobid",IF('[1]Tabelle 1'!L3=G2,"ParsCit",IF('[1]Tabelle 1'!M3=G2,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3">
+        <f>MAX('[1]Tabelle 1'!J3:M3)</f>
+        <v>91</v>
+      </c>
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="G2">
-        <f>COUNTIF(B$2:B$21,$F2)</f>
+      <c r="J2">
+        <f>COUNTIF(B$2:B$21,$I2)</f>
         <v>3</v>
       </c>
-      <c r="H2">
-        <f t="shared" ref="H2:I2" si="0">COUNTIF(C$2:C$21,$F2)</f>
+      <c r="K2">
+        <f>COUNTIF(D$2:D$21,$I2)</f>
         <v>9</v>
       </c>
-      <c r="I2">
-        <f t="shared" si="0"/>
+      <c r="L2">
+        <f>COUNTIF(F$2:F$21,$I2)</f>
         <v>4</v>
       </c>
-      <c r="J2">
-        <f>SUM(G2:I2)</f>
+      <c r="M2">
+        <f>SUM(J2:L2)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>'[1]Tabelle 1'!A4</f>
         <v>Abstract</v>
       </c>
-      <c r="B3" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B4=MAX('[1]Tabelle 1'!B4:E4),"Cermine",IF('[1]Tabelle 1'!C4=MAX('[1]Tabelle 1'!B4:E4),"Grobid",IF('[1]Tabelle 1'!D4=MAX('[1]Tabelle 1'!B4:E4),"ParsCit",IF('[1]Tabelle 1'!E4=MAX('[1]Tabelle 1'!B4:E4),"PDFX","none"))))</f>
+      <c r="B3" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B4=C3,"Cermine",IF('[1]Tabelle 1'!C4=C3,"Grobid",IF('[1]Tabelle 1'!D4=C3,"ParsCit",IF('[1]Tabelle 1'!E4=C3,"PDFX","none"))))</f>
         <v>PDFX</v>
       </c>
-      <c r="C3" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F4=MAX('[1]Tabelle 1'!F4:I4),"Cermine",IF('[1]Tabelle 1'!G4=MAX('[1]Tabelle 1'!F4:I4),"Grobid",IF('[1]Tabelle 1'!H4=MAX('[1]Tabelle 1'!F4:I4),"ParsCit",IF('[1]Tabelle 1'!I4=MAX('[1]Tabelle 1'!F4:I4),"PDFX","none"))))</f>
+      <c r="C3" s="3">
+        <f>MAX('[1]Tabelle 1'!B4:E4)</f>
+        <v>83.1</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F4=E3,"Cermine",IF('[1]Tabelle 1'!G4=E3,"Grobid",IF('[1]Tabelle 1'!H4=E3,"ParsCit",IF('[1]Tabelle 1'!I4=E3,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D3" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J4=MAX('[1]Tabelle 1'!J4:M4),"Cermine",IF('[1]Tabelle 1'!K4=MAX('[1]Tabelle 1'!J4:M4),"Grobid",IF('[1]Tabelle 1'!L4=MAX('[1]Tabelle 1'!J4:M4),"ParsCit",IF('[1]Tabelle 1'!M4=MAX('[1]Tabelle 1'!J4:M4),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="3">
+        <f>MAX('[1]Tabelle 1'!F4:I4)</f>
+        <v>69.569999999999993</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J4=G3,"Cermine",IF('[1]Tabelle 1'!K4=G3,"Grobid",IF('[1]Tabelle 1'!L4=G3,"ParsCit",IF('[1]Tabelle 1'!M4=G3,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G3" s="3">
+        <f>MAX('[1]Tabelle 1'!J4:M4)</f>
+        <v>67.39</v>
+      </c>
+      <c r="I3" t="s">
         <v>1</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G5" si="1">COUNTIF(B$2:B$21,$F3)</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">COUNTIF(B$2:B$21,$I3)</f>
         <v>14</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H5" si="2">COUNTIF(C$2:C$21,$F3)</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K5" si="1">COUNTIF(D$2:D$21,$I3)</f>
         <v>11</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I5" si="3">COUNTIF(D$2:D$21,$F3)</f>
+      <c r="L3">
+        <f t="shared" ref="L3:L5" si="2">COUNTIF(F$2:F$21,$I3)</f>
         <v>15</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J5" si="4">SUM(G3:I3)</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M5" si="3">SUM(J3:L3)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>'[1]Tabelle 1'!A5</f>
         <v>Abstract (german)</v>
       </c>
-      <c r="B4" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B5=MAX('[1]Tabelle 1'!B5:E5),"Cermine",IF('[1]Tabelle 1'!C5=MAX('[1]Tabelle 1'!B5:E5),"Grobid",IF('[1]Tabelle 1'!D5=MAX('[1]Tabelle 1'!B5:E5),"ParsCit",IF('[1]Tabelle 1'!E5=MAX('[1]Tabelle 1'!B5:E5),"PDFX","none"))))</f>
+      <c r="B4" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B5=C4,"Cermine",IF('[1]Tabelle 1'!C5=C4,"Grobid",IF('[1]Tabelle 1'!D5=C4,"ParsCit",IF('[1]Tabelle 1'!E5=C4,"PDFX","none"))))</f>
         <v>none</v>
       </c>
-      <c r="C4" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F5=MAX('[1]Tabelle 1'!F5:I5),"Cermine",IF('[1]Tabelle 1'!G5=MAX('[1]Tabelle 1'!F5:I5),"Grobid",IF('[1]Tabelle 1'!H5=MAX('[1]Tabelle 1'!F5:I5),"ParsCit",IF('[1]Tabelle 1'!I5=MAX('[1]Tabelle 1'!F5:I5),"PDFX","none"))))</f>
+      <c r="C4" s="3">
+        <f>MAX('[1]Tabelle 1'!B5:E5)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F5=E4,"Cermine",IF('[1]Tabelle 1'!G5=E4,"Grobid",IF('[1]Tabelle 1'!H5=E4,"ParsCit",IF('[1]Tabelle 1'!I5=E4,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D4" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J5=MAX('[1]Tabelle 1'!J5:M5),"Cermine",IF('[1]Tabelle 1'!K5=MAX('[1]Tabelle 1'!J5:M5),"Grobid",IF('[1]Tabelle 1'!L5=MAX('[1]Tabelle 1'!J5:M5),"ParsCit",IF('[1]Tabelle 1'!M5=MAX('[1]Tabelle 1'!J5:M5),"PDFX","none"))))</f>
+      <c r="E4" s="3">
+        <f>MAX('[1]Tabelle 1'!F5:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J5=G4,"Cermine",IF('[1]Tabelle 1'!K5=G4,"Grobid",IF('[1]Tabelle 1'!L5=G4,"ParsCit",IF('[1]Tabelle 1'!M5=G4,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="3">
+        <f>MAX('[1]Tabelle 1'!J5:M5)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I4">
+      <c r="M4">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>'[1]Tabelle 1'!A6</f>
         <v>Keywords</v>
       </c>
-      <c r="B5" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B6=MAX('[1]Tabelle 1'!B6:E6),"Cermine",IF('[1]Tabelle 1'!C6=MAX('[1]Tabelle 1'!B6:E6),"Grobid",IF('[1]Tabelle 1'!D6=MAX('[1]Tabelle 1'!B6:E6),"ParsCit",IF('[1]Tabelle 1'!E6=MAX('[1]Tabelle 1'!B6:E6),"PDFX","none"))))</f>
+      <c r="B5" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B6=C5,"Cermine",IF('[1]Tabelle 1'!C6=C5,"Grobid",IF('[1]Tabelle 1'!D6=C5,"ParsCit",IF('[1]Tabelle 1'!E6=C5,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="C5" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F6=MAX('[1]Tabelle 1'!F6:I6),"Cermine",IF('[1]Tabelle 1'!G6=MAX('[1]Tabelle 1'!F6:I6),"Grobid",IF('[1]Tabelle 1'!H6=MAX('[1]Tabelle 1'!F6:I6),"ParsCit",IF('[1]Tabelle 1'!I6=MAX('[1]Tabelle 1'!F6:I6),"PDFX","none"))))</f>
+      <c r="C5" s="3">
+        <f>MAX('[1]Tabelle 1'!B6:E6)</f>
+        <v>84.67</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F6=E5,"Cermine",IF('[1]Tabelle 1'!G6=E5,"Grobid",IF('[1]Tabelle 1'!H6=E5,"ParsCit",IF('[1]Tabelle 1'!I6=E5,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D5" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J6=MAX('[1]Tabelle 1'!J6:M6),"Cermine",IF('[1]Tabelle 1'!K6=MAX('[1]Tabelle 1'!J6:M6),"Grobid",IF('[1]Tabelle 1'!L6=MAX('[1]Tabelle 1'!J6:M6),"ParsCit",IF('[1]Tabelle 1'!M6=MAX('[1]Tabelle 1'!J6:M6),"PDFX","none"))))</f>
+      <c r="E5" s="3">
+        <f>MAX('[1]Tabelle 1'!F6:I6)</f>
+        <v>67.959999999999994</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J6=G5,"Cermine",IF('[1]Tabelle 1'!K6=G5,"Grobid",IF('[1]Tabelle 1'!L6=G5,"ParsCit",IF('[1]Tabelle 1'!M6=G5,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="3">
+        <f>MAX('[1]Tabelle 1'!J6:M6)</f>
+        <v>63.97</v>
+      </c>
+      <c r="I5" t="s">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="M5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>'[1]Tabelle 1'!A7</f>
         <v>Authors</v>
       </c>
-      <c r="B6" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B7=MAX('[1]Tabelle 1'!B7:E7),"Cermine",IF('[1]Tabelle 1'!C7=MAX('[1]Tabelle 1'!B7:E7),"Grobid",IF('[1]Tabelle 1'!D7=MAX('[1]Tabelle 1'!B7:E7),"ParsCit",IF('[1]Tabelle 1'!E7=MAX('[1]Tabelle 1'!B7:E7),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F7=MAX('[1]Tabelle 1'!F7:I7),"Cermine",IF('[1]Tabelle 1'!G7=MAX('[1]Tabelle 1'!F7:I7),"Grobid",IF('[1]Tabelle 1'!H7=MAX('[1]Tabelle 1'!F7:I7),"ParsCit",IF('[1]Tabelle 1'!I7=MAX('[1]Tabelle 1'!F7:I7),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J7=MAX('[1]Tabelle 1'!J7:M7),"Cermine",IF('[1]Tabelle 1'!K7=MAX('[1]Tabelle 1'!J7:M7),"Grobid",IF('[1]Tabelle 1'!L7=MAX('[1]Tabelle 1'!J7:M7),"ParsCit",IF('[1]Tabelle 1'!M7=MAX('[1]Tabelle 1'!J7:M7),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B7=C6,"Cermine",IF('[1]Tabelle 1'!C7=C6,"Grobid",IF('[1]Tabelle 1'!D7=C6,"ParsCit",IF('[1]Tabelle 1'!E7=C6,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C6" s="3">
+        <f>MAX('[1]Tabelle 1'!B7:E7)</f>
+        <v>85.58</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F7=E6,"Cermine",IF('[1]Tabelle 1'!G7=E6,"Grobid",IF('[1]Tabelle 1'!H7=E6,"ParsCit",IF('[1]Tabelle 1'!I7=E6,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E6" s="3">
+        <f>MAX('[1]Tabelle 1'!F7:I7)</f>
+        <v>89.35</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J7=G6,"Cermine",IF('[1]Tabelle 1'!K7=G6,"Grobid",IF('[1]Tabelle 1'!L7=G6,"ParsCit",IF('[1]Tabelle 1'!M7=G6,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G6" s="3">
+        <f>MAX('[1]Tabelle 1'!J7:M7)</f>
+        <v>84.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>'[1]Tabelle 1'!A8</f>
         <v>Emails</v>
       </c>
-      <c r="B7" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B8=MAX('[1]Tabelle 1'!B8:E8),"Cermine",IF('[1]Tabelle 1'!C8=MAX('[1]Tabelle 1'!B8:E8),"Grobid",IF('[1]Tabelle 1'!D8=MAX('[1]Tabelle 1'!B8:E8),"ParsCit",IF('[1]Tabelle 1'!E8=MAX('[1]Tabelle 1'!B8:E8),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C7" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F8=MAX('[1]Tabelle 1'!F8:I8),"Cermine",IF('[1]Tabelle 1'!G8=MAX('[1]Tabelle 1'!F8:I8),"Grobid",IF('[1]Tabelle 1'!H8=MAX('[1]Tabelle 1'!F8:I8),"ParsCit",IF('[1]Tabelle 1'!I8=MAX('[1]Tabelle 1'!F8:I8),"PDFX","none"))))</f>
+      <c r="B7" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B8=C7,"Cermine",IF('[1]Tabelle 1'!C8=C7,"Grobid",IF('[1]Tabelle 1'!D8=C7,"ParsCit",IF('[1]Tabelle 1'!E8=C7,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C7" s="3">
+        <f>MAX('[1]Tabelle 1'!B8:E8)</f>
+        <v>90.32</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F8=E7,"Cermine",IF('[1]Tabelle 1'!G8=E7,"Grobid",IF('[1]Tabelle 1'!H8=E7,"ParsCit",IF('[1]Tabelle 1'!I8=E7,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D7" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J8=MAX('[1]Tabelle 1'!J8:M8),"Cermine",IF('[1]Tabelle 1'!K8=MAX('[1]Tabelle 1'!J8:M8),"Grobid",IF('[1]Tabelle 1'!L8=MAX('[1]Tabelle 1'!J8:M8),"ParsCit",IF('[1]Tabelle 1'!M8=MAX('[1]Tabelle 1'!J8:M8),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" s="3">
+        <f>MAX('[1]Tabelle 1'!F8:I8)</f>
+        <v>70.650000000000006</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J8=G7,"Cermine",IF('[1]Tabelle 1'!K8=G7,"Grobid",IF('[1]Tabelle 1'!L8=G7,"ParsCit",IF('[1]Tabelle 1'!M8=G7,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G7" s="3">
+        <f>MAX('[1]Tabelle 1'!J8:M8)</f>
+        <v>63.69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>'[1]Tabelle 1'!A9</f>
         <v>Author-Emails</v>
       </c>
-      <c r="B8" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B9=MAX('[1]Tabelle 1'!B9:E9),"Cermine",IF('[1]Tabelle 1'!C9=MAX('[1]Tabelle 1'!B9:E9),"Grobid",IF('[1]Tabelle 1'!D9=MAX('[1]Tabelle 1'!B9:E9),"ParsCit",IF('[1]Tabelle 1'!E9=MAX('[1]Tabelle 1'!B9:E9),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F9=MAX('[1]Tabelle 1'!F9:I9),"Cermine",IF('[1]Tabelle 1'!G9=MAX('[1]Tabelle 1'!F9:I9),"Grobid",IF('[1]Tabelle 1'!H9=MAX('[1]Tabelle 1'!F9:I9),"ParsCit",IF('[1]Tabelle 1'!I9=MAX('[1]Tabelle 1'!F9:I9),"PDFX","none"))))</f>
+      <c r="B8" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B9=C8,"Cermine",IF('[1]Tabelle 1'!C9=C8,"Grobid",IF('[1]Tabelle 1'!D9=C8,"ParsCit",IF('[1]Tabelle 1'!E9=C8,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C8" s="3">
+        <f>MAX('[1]Tabelle 1'!B9:E9)</f>
+        <v>85.59</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F9=E8,"Cermine",IF('[1]Tabelle 1'!G9=E8,"Grobid",IF('[1]Tabelle 1'!H9=E8,"ParsCit",IF('[1]Tabelle 1'!I9=E8,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D8" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J9=MAX('[1]Tabelle 1'!J9:M9),"Cermine",IF('[1]Tabelle 1'!K9=MAX('[1]Tabelle 1'!J9:M9),"Grobid",IF('[1]Tabelle 1'!L9=MAX('[1]Tabelle 1'!J9:M9),"ParsCit",IF('[1]Tabelle 1'!M9=MAX('[1]Tabelle 1'!J9:M9),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E8" s="3">
+        <f>MAX('[1]Tabelle 1'!F9:I9)</f>
+        <v>66.67</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J9=G8,"Cermine",IF('[1]Tabelle 1'!K9=G8,"Grobid",IF('[1]Tabelle 1'!L9=G8,"ParsCit",IF('[1]Tabelle 1'!M9=G8,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G8" s="3">
+        <f>MAX('[1]Tabelle 1'!J9:M9)</f>
+        <v>60.07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>'[1]Tabelle 1'!A10</f>
         <v>Affiliations</v>
       </c>
-      <c r="B9" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B10=MAX('[1]Tabelle 1'!B10:E10),"Cermine",IF('[1]Tabelle 1'!C10=MAX('[1]Tabelle 1'!B10:E10),"Grobid",IF('[1]Tabelle 1'!D10=MAX('[1]Tabelle 1'!B10:E10),"ParsCit",IF('[1]Tabelle 1'!E10=MAX('[1]Tabelle 1'!B10:E10),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C9" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F10=MAX('[1]Tabelle 1'!F10:I10),"Cermine",IF('[1]Tabelle 1'!G10=MAX('[1]Tabelle 1'!F10:I10),"Grobid",IF('[1]Tabelle 1'!H10=MAX('[1]Tabelle 1'!F10:I10),"ParsCit",IF('[1]Tabelle 1'!I10=MAX('[1]Tabelle 1'!F10:I10),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D9" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J10=MAX('[1]Tabelle 1'!J10:M10),"Cermine",IF('[1]Tabelle 1'!K10=MAX('[1]Tabelle 1'!J10:M10),"Grobid",IF('[1]Tabelle 1'!L10=MAX('[1]Tabelle 1'!J10:M10),"ParsCit",IF('[1]Tabelle 1'!M10=MAX('[1]Tabelle 1'!J10:M10),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B10=C9,"Cermine",IF('[1]Tabelle 1'!C10=C9,"Grobid",IF('[1]Tabelle 1'!D10=C9,"ParsCit",IF('[1]Tabelle 1'!E10=C9,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C9" s="3">
+        <f>MAX('[1]Tabelle 1'!B10:E10)</f>
+        <v>89.29</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F10=E9,"Cermine",IF('[1]Tabelle 1'!G10=E9,"Grobid",IF('[1]Tabelle 1'!H10=E9,"ParsCit",IF('[1]Tabelle 1'!I10=E9,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E9" s="3">
+        <f>MAX('[1]Tabelle 1'!F10:I10)</f>
+        <v>82.68</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J10=G9,"Cermine",IF('[1]Tabelle 1'!K10=G9,"Grobid",IF('[1]Tabelle 1'!L10=G9,"ParsCit",IF('[1]Tabelle 1'!M10=G9,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G9" s="3">
+        <f>MAX('[1]Tabelle 1'!J10:M10)</f>
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>'[1]Tabelle 1'!A11</f>
         <v>Author-Affiliations</v>
       </c>
-      <c r="B10" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B11=MAX('[1]Tabelle 1'!B11:E11),"Cermine",IF('[1]Tabelle 1'!C11=MAX('[1]Tabelle 1'!B11:E11),"Grobid",IF('[1]Tabelle 1'!D11=MAX('[1]Tabelle 1'!B11:E11),"ParsCit",IF('[1]Tabelle 1'!E11=MAX('[1]Tabelle 1'!B11:E11),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C10" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F11=MAX('[1]Tabelle 1'!F11:I11),"Cermine",IF('[1]Tabelle 1'!G11=MAX('[1]Tabelle 1'!F11:I11),"Grobid",IF('[1]Tabelle 1'!H11=MAX('[1]Tabelle 1'!F11:I11),"ParsCit",IF('[1]Tabelle 1'!I11=MAX('[1]Tabelle 1'!F11:I11),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J11=MAX('[1]Tabelle 1'!J11:M11),"Cermine",IF('[1]Tabelle 1'!K11=MAX('[1]Tabelle 1'!J11:M11),"Grobid",IF('[1]Tabelle 1'!L11=MAX('[1]Tabelle 1'!J11:M11),"ParsCit",IF('[1]Tabelle 1'!M11=MAX('[1]Tabelle 1'!J11:M11),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B11=C10,"Cermine",IF('[1]Tabelle 1'!C11=C10,"Grobid",IF('[1]Tabelle 1'!D11=C10,"ParsCit",IF('[1]Tabelle 1'!E11=C10,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C10" s="3">
+        <f>MAX('[1]Tabelle 1'!B11:E11)</f>
+        <v>65.89</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F11=E10,"Cermine",IF('[1]Tabelle 1'!G11=E10,"Grobid",IF('[1]Tabelle 1'!H11=E10,"ParsCit",IF('[1]Tabelle 1'!I11=E10,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E10" s="3">
+        <f>MAX('[1]Tabelle 1'!F11:I11)</f>
+        <v>69.599999999999994</v>
+      </c>
+      <c r="F10" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J11=G10,"Cermine",IF('[1]Tabelle 1'!K11=G10,"Grobid",IF('[1]Tabelle 1'!L11=G10,"ParsCit",IF('[1]Tabelle 1'!M11=G10,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G10" s="3">
+        <f>MAX('[1]Tabelle 1'!J11:M11)</f>
+        <v>64.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>'[1]Tabelle 1'!A12</f>
         <v>Source</v>
       </c>
-      <c r="B11" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B12=MAX('[1]Tabelle 1'!B12:E12),"Cermine",IF('[1]Tabelle 1'!C12=MAX('[1]Tabelle 1'!B12:E12),"Grobid",IF('[1]Tabelle 1'!D12=MAX('[1]Tabelle 1'!B12:E12),"ParsCit",IF('[1]Tabelle 1'!E12=MAX('[1]Tabelle 1'!B12:E12),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C11" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F12=MAX('[1]Tabelle 1'!F12:I12),"Cermine",IF('[1]Tabelle 1'!G12=MAX('[1]Tabelle 1'!F12:I12),"Grobid",IF('[1]Tabelle 1'!H12=MAX('[1]Tabelle 1'!F12:I12),"ParsCit",IF('[1]Tabelle 1'!I12=MAX('[1]Tabelle 1'!F12:I12),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D11" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J12=MAX('[1]Tabelle 1'!J12:M12),"Cermine",IF('[1]Tabelle 1'!K12=MAX('[1]Tabelle 1'!J12:M12),"Grobid",IF('[1]Tabelle 1'!L12=MAX('[1]Tabelle 1'!J12:M12),"ParsCit",IF('[1]Tabelle 1'!M12=MAX('[1]Tabelle 1'!J12:M12),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B12=C11,"Cermine",IF('[1]Tabelle 1'!C12=C11,"Grobid",IF('[1]Tabelle 1'!D12=C11,"ParsCit",IF('[1]Tabelle 1'!E12=C11,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C11" s="3">
+        <f>MAX('[1]Tabelle 1'!B12:E12)</f>
+        <v>66.67</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F12=E11,"Cermine",IF('[1]Tabelle 1'!G12=E11,"Grobid",IF('[1]Tabelle 1'!H12=E11,"ParsCit",IF('[1]Tabelle 1'!I12=E11,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E11" s="3">
+        <f>MAX('[1]Tabelle 1'!F12:I12)</f>
+        <v>21.05</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J12=G11,"Cermine",IF('[1]Tabelle 1'!K12=G11,"Grobid",IF('[1]Tabelle 1'!L12=G11,"ParsCit",IF('[1]Tabelle 1'!M12=G11,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G11" s="3">
+        <f>MAX('[1]Tabelle 1'!J12:M12)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>'[1]Tabelle 1'!A13</f>
         <v>Volume</v>
       </c>
-      <c r="B12" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B13=MAX('[1]Tabelle 1'!B13:E13),"Cermine",IF('[1]Tabelle 1'!C13=MAX('[1]Tabelle 1'!B13:E13),"Grobid",IF('[1]Tabelle 1'!D13=MAX('[1]Tabelle 1'!B13:E13),"ParsCit",IF('[1]Tabelle 1'!E13=MAX('[1]Tabelle 1'!B13:E13),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F13=MAX('[1]Tabelle 1'!F13:I13),"Cermine",IF('[1]Tabelle 1'!G13=MAX('[1]Tabelle 1'!F13:I13),"Grobid",IF('[1]Tabelle 1'!H13=MAX('[1]Tabelle 1'!F13:I13),"ParsCit",IF('[1]Tabelle 1'!I13=MAX('[1]Tabelle 1'!F13:I13),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J13=MAX('[1]Tabelle 1'!J13:M13),"Cermine",IF('[1]Tabelle 1'!K13=MAX('[1]Tabelle 1'!J13:M13),"Grobid",IF('[1]Tabelle 1'!L13=MAX('[1]Tabelle 1'!J13:M13),"ParsCit",IF('[1]Tabelle 1'!M13=MAX('[1]Tabelle 1'!J13:M13),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B13=C12,"Cermine",IF('[1]Tabelle 1'!C13=C12,"Grobid",IF('[1]Tabelle 1'!D13=C12,"ParsCit",IF('[1]Tabelle 1'!E13=C12,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C12" s="3">
+        <f>MAX('[1]Tabelle 1'!B13:E13)</f>
+        <v>100</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F13=E12,"Cermine",IF('[1]Tabelle 1'!G13=E12,"Grobid",IF('[1]Tabelle 1'!H13=E12,"ParsCit",IF('[1]Tabelle 1'!I13=E12,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E12" s="3">
+        <f>MAX('[1]Tabelle 1'!F13:I13)</f>
+        <v>100</v>
+      </c>
+      <c r="F12" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J13=G12,"Cermine",IF('[1]Tabelle 1'!K13=G12,"Grobid",IF('[1]Tabelle 1'!L13=G12,"ParsCit",IF('[1]Tabelle 1'!M13=G12,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G12" s="3">
+        <f>MAX('[1]Tabelle 1'!J13:M13)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f>'[1]Tabelle 1'!A14</f>
         <v>Issue</v>
       </c>
-      <c r="B13" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B14=MAX('[1]Tabelle 1'!B14:E14),"Cermine",IF('[1]Tabelle 1'!C14=MAX('[1]Tabelle 1'!B14:E14),"Grobid",IF('[1]Tabelle 1'!D14=MAX('[1]Tabelle 1'!B14:E14),"ParsCit",IF('[1]Tabelle 1'!E14=MAX('[1]Tabelle 1'!B14:E14),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C13" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F14=MAX('[1]Tabelle 1'!F14:I14),"Cermine",IF('[1]Tabelle 1'!G14=MAX('[1]Tabelle 1'!F14:I14),"Grobid",IF('[1]Tabelle 1'!H14=MAX('[1]Tabelle 1'!F14:I14),"ParsCit",IF('[1]Tabelle 1'!I14=MAX('[1]Tabelle 1'!F14:I14),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D13" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J14=MAX('[1]Tabelle 1'!J14:M14),"Cermine",IF('[1]Tabelle 1'!K14=MAX('[1]Tabelle 1'!J14:M14),"Grobid",IF('[1]Tabelle 1'!L14=MAX('[1]Tabelle 1'!J14:M14),"ParsCit",IF('[1]Tabelle 1'!M14=MAX('[1]Tabelle 1'!J14:M14),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B14=C13,"Cermine",IF('[1]Tabelle 1'!C14=C13,"Grobid",IF('[1]Tabelle 1'!D14=C13,"ParsCit",IF('[1]Tabelle 1'!E14=C13,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C13" s="3">
+        <f>MAX('[1]Tabelle 1'!B14:E14)</f>
+        <v>100</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F14=E13,"Cermine",IF('[1]Tabelle 1'!G14=E13,"Grobid",IF('[1]Tabelle 1'!H14=E13,"ParsCit",IF('[1]Tabelle 1'!I14=E13,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E13" s="3">
+        <f>MAX('[1]Tabelle 1'!F14:I14)</f>
+        <v>100</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J14=G13,"Cermine",IF('[1]Tabelle 1'!K14=G13,"Grobid",IF('[1]Tabelle 1'!L14=G13,"ParsCit",IF('[1]Tabelle 1'!M14=G13,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G13" s="3">
+        <f>MAX('[1]Tabelle 1'!J14:M14)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f>'[1]Tabelle 1'!A15</f>
         <v>Page from</v>
       </c>
-      <c r="B14" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B15=MAX('[1]Tabelle 1'!B15:E15),"Cermine",IF('[1]Tabelle 1'!C15=MAX('[1]Tabelle 1'!B15:E15),"Grobid",IF('[1]Tabelle 1'!D15=MAX('[1]Tabelle 1'!B15:E15),"ParsCit",IF('[1]Tabelle 1'!E15=MAX('[1]Tabelle 1'!B15:E15),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F15=MAX('[1]Tabelle 1'!F15:I15),"Cermine",IF('[1]Tabelle 1'!G15=MAX('[1]Tabelle 1'!F15:I15),"Grobid",IF('[1]Tabelle 1'!H15=MAX('[1]Tabelle 1'!F15:I15),"ParsCit",IF('[1]Tabelle 1'!I15=MAX('[1]Tabelle 1'!F15:I15),"PDFX","none"))))</f>
+      <c r="B14" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B15=C14,"Cermine",IF('[1]Tabelle 1'!C15=C14,"Grobid",IF('[1]Tabelle 1'!D15=C14,"ParsCit",IF('[1]Tabelle 1'!E15=C14,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C14" s="3">
+        <f>MAX('[1]Tabelle 1'!B15:E15)</f>
+        <v>100</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F15=E14,"Cermine",IF('[1]Tabelle 1'!G15=E14,"Grobid",IF('[1]Tabelle 1'!H15=E14,"ParsCit",IF('[1]Tabelle 1'!I15=E14,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D14" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J15=MAX('[1]Tabelle 1'!J15:M15),"Cermine",IF('[1]Tabelle 1'!K15=MAX('[1]Tabelle 1'!J15:M15),"Grobid",IF('[1]Tabelle 1'!L15=MAX('[1]Tabelle 1'!J15:M15),"ParsCit",IF('[1]Tabelle 1'!M15=MAX('[1]Tabelle 1'!J15:M15),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14" s="3">
+        <f>MAX('[1]Tabelle 1'!F15:I15)</f>
+        <v>100</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J15=G14,"Cermine",IF('[1]Tabelle 1'!K15=G14,"Grobid",IF('[1]Tabelle 1'!L15=G14,"ParsCit",IF('[1]Tabelle 1'!M15=G14,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G14" s="3">
+        <f>MAX('[1]Tabelle 1'!J15:M15)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f>'[1]Tabelle 1'!A16</f>
         <v>Page to</v>
       </c>
-      <c r="B15" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B16=MAX('[1]Tabelle 1'!B16:E16),"Cermine",IF('[1]Tabelle 1'!C16=MAX('[1]Tabelle 1'!B16:E16),"Grobid",IF('[1]Tabelle 1'!D16=MAX('[1]Tabelle 1'!B16:E16),"ParsCit",IF('[1]Tabelle 1'!E16=MAX('[1]Tabelle 1'!B16:E16),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C15" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F16=MAX('[1]Tabelle 1'!F16:I16),"Cermine",IF('[1]Tabelle 1'!G16=MAX('[1]Tabelle 1'!F16:I16),"Grobid",IF('[1]Tabelle 1'!H16=MAX('[1]Tabelle 1'!F16:I16),"ParsCit",IF('[1]Tabelle 1'!I16=MAX('[1]Tabelle 1'!F16:I16),"PDFX","none"))))</f>
+      <c r="B15" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B16=C15,"Cermine",IF('[1]Tabelle 1'!C16=C15,"Grobid",IF('[1]Tabelle 1'!D16=C15,"ParsCit",IF('[1]Tabelle 1'!E16=C15,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C15" s="3">
+        <f>MAX('[1]Tabelle 1'!B16:E16)</f>
+        <v>100</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F16=E15,"Cermine",IF('[1]Tabelle 1'!G16=E15,"Grobid",IF('[1]Tabelle 1'!H16=E15,"ParsCit",IF('[1]Tabelle 1'!I16=E15,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D15" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J16=MAX('[1]Tabelle 1'!J16:M16),"Cermine",IF('[1]Tabelle 1'!K16=MAX('[1]Tabelle 1'!J16:M16),"Grobid",IF('[1]Tabelle 1'!L16=MAX('[1]Tabelle 1'!J16:M16),"ParsCit",IF('[1]Tabelle 1'!M16=MAX('[1]Tabelle 1'!J16:M16),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E15" s="3">
+        <f>MAX('[1]Tabelle 1'!F16:I16)</f>
+        <v>100</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J16=G15,"Cermine",IF('[1]Tabelle 1'!K16=G15,"Grobid",IF('[1]Tabelle 1'!L16=G15,"ParsCit",IF('[1]Tabelle 1'!M16=G15,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G15" s="3">
+        <f>MAX('[1]Tabelle 1'!J16:M16)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f>'[1]Tabelle 1'!A17</f>
         <v>Year</v>
       </c>
-      <c r="B16" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B17=MAX('[1]Tabelle 1'!B17:E17),"Cermine",IF('[1]Tabelle 1'!C17=MAX('[1]Tabelle 1'!B17:E17),"Grobid",IF('[1]Tabelle 1'!D17=MAX('[1]Tabelle 1'!B17:E17),"ParsCit",IF('[1]Tabelle 1'!E17=MAX('[1]Tabelle 1'!B17:E17),"PDFX","none"))))</f>
+      <c r="B16" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B17=C16,"Cermine",IF('[1]Tabelle 1'!C17=C16,"Grobid",IF('[1]Tabelle 1'!D17=C16,"ParsCit",IF('[1]Tabelle 1'!E17=C16,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="C16" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F17=MAX('[1]Tabelle 1'!F17:I17),"Cermine",IF('[1]Tabelle 1'!G17=MAX('[1]Tabelle 1'!F17:I17),"Grobid",IF('[1]Tabelle 1'!H17=MAX('[1]Tabelle 1'!F17:I17),"ParsCit",IF('[1]Tabelle 1'!I17=MAX('[1]Tabelle 1'!F17:I17),"PDFX","none"))))</f>
+      <c r="C16" s="3">
+        <f>MAX('[1]Tabelle 1'!B17:E17)</f>
+        <v>48.84</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F17=E16,"Cermine",IF('[1]Tabelle 1'!G17=E16,"Grobid",IF('[1]Tabelle 1'!H17=E16,"ParsCit",IF('[1]Tabelle 1'!I17=E16,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="D16" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J17=MAX('[1]Tabelle 1'!J17:M17),"Cermine",IF('[1]Tabelle 1'!K17=MAX('[1]Tabelle 1'!J17:M17),"Grobid",IF('[1]Tabelle 1'!L17=MAX('[1]Tabelle 1'!J17:M17),"ParsCit",IF('[1]Tabelle 1'!M17=MAX('[1]Tabelle 1'!J17:M17),"PDFX","none"))))</f>
+      <c r="E16" s="3">
+        <f>MAX('[1]Tabelle 1'!F17:I17)</f>
+        <v>65.63</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J17=G16,"Cermine",IF('[1]Tabelle 1'!K17=G16,"Grobid",IF('[1]Tabelle 1'!L17=G16,"ParsCit",IF('[1]Tabelle 1'!M17=G16,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16" s="3">
+        <f>MAX('[1]Tabelle 1'!J17:M17)</f>
+        <v>46.67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f>'[1]Tabelle 1'!A18</f>
         <v>Doi</v>
       </c>
-      <c r="B17" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B18=MAX('[1]Tabelle 1'!B18:E18),"Cermine",IF('[1]Tabelle 1'!C18=MAX('[1]Tabelle 1'!B18:E18),"Grobid",IF('[1]Tabelle 1'!D18=MAX('[1]Tabelle 1'!B18:E18),"ParsCit",IF('[1]Tabelle 1'!E18=MAX('[1]Tabelle 1'!B18:E18),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C17" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F18=MAX('[1]Tabelle 1'!F18:I18),"Cermine",IF('[1]Tabelle 1'!G18=MAX('[1]Tabelle 1'!F18:I18),"Grobid",IF('[1]Tabelle 1'!H18=MAX('[1]Tabelle 1'!F18:I18),"ParsCit",IF('[1]Tabelle 1'!I18=MAX('[1]Tabelle 1'!F18:I18),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D17" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J18=MAX('[1]Tabelle 1'!J18:M18),"Cermine",IF('[1]Tabelle 1'!K18=MAX('[1]Tabelle 1'!J18:M18),"Grobid",IF('[1]Tabelle 1'!L18=MAX('[1]Tabelle 1'!J18:M18),"ParsCit",IF('[1]Tabelle 1'!M18=MAX('[1]Tabelle 1'!J18:M18),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B18=C17,"Cermine",IF('[1]Tabelle 1'!C18=C17,"Grobid",IF('[1]Tabelle 1'!D18=C17,"ParsCit",IF('[1]Tabelle 1'!E18=C17,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C17" s="3">
+        <f>MAX('[1]Tabelle 1'!B18:E18)</f>
+        <v>100</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F18=E17,"Cermine",IF('[1]Tabelle 1'!G18=E17,"Grobid",IF('[1]Tabelle 1'!H18=E17,"ParsCit",IF('[1]Tabelle 1'!I18=E17,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E17" s="3">
+        <f>MAX('[1]Tabelle 1'!F18:I18)</f>
+        <v>100</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J18=G17,"Cermine",IF('[1]Tabelle 1'!K18=G17,"Grobid",IF('[1]Tabelle 1'!L18=G17,"ParsCit",IF('[1]Tabelle 1'!M18=G17,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G17" s="3">
+        <f>MAX('[1]Tabelle 1'!J18:M18)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="str">
         <f>'[1]Tabelle 1'!A19</f>
         <v>Sections</v>
       </c>
-      <c r="B18" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B19=MAX('[1]Tabelle 1'!B19:E19),"Cermine",IF('[1]Tabelle 1'!C19=MAX('[1]Tabelle 1'!B19:E19),"Grobid",IF('[1]Tabelle 1'!D19=MAX('[1]Tabelle 1'!B19:E19),"ParsCit",IF('[1]Tabelle 1'!E19=MAX('[1]Tabelle 1'!B19:E19),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F19=MAX('[1]Tabelle 1'!F19:I19),"Cermine",IF('[1]Tabelle 1'!G19=MAX('[1]Tabelle 1'!F19:I19),"Grobid",IF('[1]Tabelle 1'!H19=MAX('[1]Tabelle 1'!F19:I19),"ParsCit",IF('[1]Tabelle 1'!I19=MAX('[1]Tabelle 1'!F19:I19),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J19=MAX('[1]Tabelle 1'!J19:M19),"Cermine",IF('[1]Tabelle 1'!K19=MAX('[1]Tabelle 1'!J19:M19),"Grobid",IF('[1]Tabelle 1'!L19=MAX('[1]Tabelle 1'!J19:M19),"ParsCit",IF('[1]Tabelle 1'!M19=MAX('[1]Tabelle 1'!J19:M19),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B19=C18,"Cermine",IF('[1]Tabelle 1'!C19=C18,"Grobid",IF('[1]Tabelle 1'!D19=C18,"ParsCit",IF('[1]Tabelle 1'!E19=C18,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C18" s="3">
+        <f>MAX('[1]Tabelle 1'!B19:E19)</f>
+        <v>83.45</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F19=E18,"Cermine",IF('[1]Tabelle 1'!G19=E18,"Grobid",IF('[1]Tabelle 1'!H19=E18,"ParsCit",IF('[1]Tabelle 1'!I19=E18,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E18" s="3">
+        <f>MAX('[1]Tabelle 1'!F19:I19)</f>
+        <v>83.95</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J19=G18,"Cermine",IF('[1]Tabelle 1'!K19=G18,"Grobid",IF('[1]Tabelle 1'!L19=G18,"ParsCit",IF('[1]Tabelle 1'!M19=G18,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G18" s="3">
+        <f>MAX('[1]Tabelle 1'!J19:M19)</f>
+        <v>81.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="str">
         <f>'[1]Tabelle 1'!A20</f>
         <v>Section-Levels</v>
       </c>
-      <c r="B19" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B20=MAX('[1]Tabelle 1'!B20:E20),"Cermine",IF('[1]Tabelle 1'!C20=MAX('[1]Tabelle 1'!B20:E20),"Grobid",IF('[1]Tabelle 1'!D20=MAX('[1]Tabelle 1'!B20:E20),"ParsCit",IF('[1]Tabelle 1'!E20=MAX('[1]Tabelle 1'!B20:E20),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C19" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F20=MAX('[1]Tabelle 1'!F20:I20),"Cermine",IF('[1]Tabelle 1'!G20=MAX('[1]Tabelle 1'!F20:I20),"Grobid",IF('[1]Tabelle 1'!H20=MAX('[1]Tabelle 1'!F20:I20),"ParsCit",IF('[1]Tabelle 1'!I20=MAX('[1]Tabelle 1'!F20:I20),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D19" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J20=MAX('[1]Tabelle 1'!J20:M20),"Cermine",IF('[1]Tabelle 1'!K20=MAX('[1]Tabelle 1'!J20:M20),"Grobid",IF('[1]Tabelle 1'!L20=MAX('[1]Tabelle 1'!J20:M20),"ParsCit",IF('[1]Tabelle 1'!M20=MAX('[1]Tabelle 1'!J20:M20),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B20=C19,"Cermine",IF('[1]Tabelle 1'!C20=C19,"Grobid",IF('[1]Tabelle 1'!D20=C19,"ParsCit",IF('[1]Tabelle 1'!E20=C19,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C19" s="3">
+        <f>MAX('[1]Tabelle 1'!B20:E20)</f>
+        <v>95.45</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F20=E19,"Cermine",IF('[1]Tabelle 1'!G20=E19,"Grobid",IF('[1]Tabelle 1'!H20=E19,"ParsCit",IF('[1]Tabelle 1'!I20=E19,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E19" s="3">
+        <f>MAX('[1]Tabelle 1'!F20:I20)</f>
+        <v>84.14</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J20=G19,"Cermine",IF('[1]Tabelle 1'!K20=G19,"Grobid",IF('[1]Tabelle 1'!L20=G19,"ParsCit",IF('[1]Tabelle 1'!M20=G19,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G19" s="3">
+        <f>MAX('[1]Tabelle 1'!J20:M20)</f>
+        <v>86.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="str">
         <f>'[1]Tabelle 1'!A21</f>
         <v>Section-References</v>
       </c>
-      <c r="B20" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B21=MAX('[1]Tabelle 1'!B21:E21),"Cermine",IF('[1]Tabelle 1'!C21=MAX('[1]Tabelle 1'!B21:E21),"Grobid",IF('[1]Tabelle 1'!D21=MAX('[1]Tabelle 1'!B21:E21),"ParsCit",IF('[1]Tabelle 1'!E21=MAX('[1]Tabelle 1'!B21:E21),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F21=MAX('[1]Tabelle 1'!F21:I21),"Cermine",IF('[1]Tabelle 1'!G21=MAX('[1]Tabelle 1'!F21:I21),"Grobid",IF('[1]Tabelle 1'!H21=MAX('[1]Tabelle 1'!F21:I21),"ParsCit",IF('[1]Tabelle 1'!I21=MAX('[1]Tabelle 1'!F21:I21),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J21=MAX('[1]Tabelle 1'!J21:M21),"Cermine",IF('[1]Tabelle 1'!K21=MAX('[1]Tabelle 1'!J21:M21),"Grobid",IF('[1]Tabelle 1'!L21=MAX('[1]Tabelle 1'!J21:M21),"ParsCit",IF('[1]Tabelle 1'!M21=MAX('[1]Tabelle 1'!J21:M21),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B21=C20,"Cermine",IF('[1]Tabelle 1'!C21=C20,"Grobid",IF('[1]Tabelle 1'!D21=C20,"ParsCit",IF('[1]Tabelle 1'!E21=C20,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C20" s="3">
+        <f>MAX('[1]Tabelle 1'!B21:E21)</f>
+        <v>62.71</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F21=E20,"Cermine",IF('[1]Tabelle 1'!G21=E20,"Grobid",IF('[1]Tabelle 1'!H21=E20,"ParsCit",IF('[1]Tabelle 1'!I21=E20,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E20" s="3">
+        <f>MAX('[1]Tabelle 1'!F21:I21)</f>
+        <v>47.77</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J21=G20,"Cermine",IF('[1]Tabelle 1'!K21=G20,"Grobid",IF('[1]Tabelle 1'!L21=G20,"ParsCit",IF('[1]Tabelle 1'!M21=G20,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G20" s="3">
+        <f>MAX('[1]Tabelle 1'!J21:M21)</f>
+        <v>48.73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="str">
         <f>'[1]Tabelle 1'!A22</f>
         <v>References</v>
       </c>
-      <c r="B21" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!B22=MAX('[1]Tabelle 1'!B22:E22),"Cermine",IF('[1]Tabelle 1'!C22=MAX('[1]Tabelle 1'!B22:E22),"Grobid",IF('[1]Tabelle 1'!D22=MAX('[1]Tabelle 1'!B22:E22),"ParsCit",IF('[1]Tabelle 1'!E22=MAX('[1]Tabelle 1'!B22:E22),"PDFX","none"))))</f>
+      <c r="B21" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B22=C21,"Cermine",IF('[1]Tabelle 1'!C22=C21,"Grobid",IF('[1]Tabelle 1'!D22=C21,"ParsCit",IF('[1]Tabelle 1'!E22=C21,"PDFX","none"))))</f>
         <v>ParsCit</v>
       </c>
-      <c r="C21" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!F22=MAX('[1]Tabelle 1'!F22:I22),"Cermine",IF('[1]Tabelle 1'!G22=MAX('[1]Tabelle 1'!F22:I22),"Grobid",IF('[1]Tabelle 1'!H22=MAX('[1]Tabelle 1'!F22:I22),"ParsCit",IF('[1]Tabelle 1'!I22=MAX('[1]Tabelle 1'!F22:I22),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D21" s="4" t="str">
-        <f>IF('[1]Tabelle 1'!J22=MAX('[1]Tabelle 1'!J22:M22),"Cermine",IF('[1]Tabelle 1'!K22=MAX('[1]Tabelle 1'!J22:M22),"Grobid",IF('[1]Tabelle 1'!L22=MAX('[1]Tabelle 1'!J22:M22),"ParsCit",IF('[1]Tabelle 1'!M22=MAX('[1]Tabelle 1'!J22:M22),"PDFX","none"))))</f>
+      <c r="C21" s="3">
+        <f>MAX('[1]Tabelle 1'!B22:E22)</f>
+        <v>97.25</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F22=E21,"Cermine",IF('[1]Tabelle 1'!G22=E21,"Grobid",IF('[1]Tabelle 1'!H22=E21,"ParsCit",IF('[1]Tabelle 1'!I22=E21,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E21" s="3">
+        <f>MAX('[1]Tabelle 1'!F22:I22)</f>
+        <v>90.93</v>
+      </c>
+      <c r="F21" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J22=G21,"Cermine",IF('[1]Tabelle 1'!K22=G21,"Grobid",IF('[1]Tabelle 1'!L22=G21,"ParsCit",IF('[1]Tabelle 1'!M22=G21,"PDFX","none"))))</f>
         <v>ParsCit</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G21" s="3">
+        <f>MAX('[1]Tabelle 1'!J22:M22)</f>
+        <v>92.44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="str">
         <f>'[1]Tabelle 1'!A23</f>
         <v>Average</v>
       </c>
-      <c r="B23" s="2" t="str">
-        <f>IF('[1]Tabelle 1'!B23=MAX('[1]Tabelle 1'!B23:E23),"Cermine",IF('[1]Tabelle 1'!C23=MAX('[1]Tabelle 1'!B23:E23),"Grobid",IF('[1]Tabelle 1'!D23=MAX('[1]Tabelle 1'!B23:E23),"ParsCit",IF('[1]Tabelle 1'!E23=MAX('[1]Tabelle 1'!B23:E23),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f>IF('[1]Tabelle 1'!F23=MAX('[1]Tabelle 1'!F23:I23),"Cermine",IF('[1]Tabelle 1'!G23=MAX('[1]Tabelle 1'!F23:I23),"Grobid",IF('[1]Tabelle 1'!H23=MAX('[1]Tabelle 1'!F23:I23),"ParsCit",IF('[1]Tabelle 1'!I23=MAX('[1]Tabelle 1'!F23:I23),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f>IF('[1]Tabelle 1'!J23=MAX('[1]Tabelle 1'!J23:M23),"Cermine",IF('[1]Tabelle 1'!K23=MAX('[1]Tabelle 1'!J23:M23),"Grobid",IF('[1]Tabelle 1'!L23=MAX('[1]Tabelle 1'!J23:M23),"ParsCit",IF('[1]Tabelle 1'!M23=MAX('[1]Tabelle 1'!J23:M23),"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="B23" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!B23=C23,"Cermine",IF('[1]Tabelle 1'!C23=C23,"Grobid",IF('[1]Tabelle 1'!D23=C23,"ParsCit",IF('[1]Tabelle 1'!E23=C23,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C23" s="3">
+        <f>MAX('[1]Tabelle 1'!B23:E23)</f>
+        <v>86.45</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!F23=E23,"Cermine",IF('[1]Tabelle 1'!G23=E23,"Grobid",IF('[1]Tabelle 1'!H23=E23,"ParsCit",IF('[1]Tabelle 1'!I23=E23,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="E23" s="3">
+        <f>MAX('[1]Tabelle 1'!F23:I23)</f>
+        <v>65.3</v>
+      </c>
+      <c r="F23" s="3" t="str">
+        <f>IF('[1]Tabelle 1'!J23=G23,"Cermine",IF('[1]Tabelle 1'!K23=G23,"Grobid",IF('[1]Tabelle 1'!L23=G23,"ParsCit",IF('[1]Tabelle 1'!M23=G23,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="G23" s="3">
+        <f>MAX('[1]Tabelle 1'!J23:M23)</f>
+        <v>64.760000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D21">
+  <conditionalFormatting sqref="B2:G21 B23:G23">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>NOT(AND(EXACT($B2,$C2),EXACT($C2,$D2)))</formula>
+      <formula>NOT(AND(EXACT($B2,$D2),EXACT($D2,$F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
statistics - adapted all-best and added grobid overview file
</commit_message>
<xml_diff>
--- a/MethodDemos/output/statistics/all-best-method-per-evaltype-publication-statistics.xlsx
+++ b/MethodDemos/output/statistics/all-best-method-per-evaltype-publication-statistics.xlsx
@@ -16,13 +16,14 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Cermine</t>
   </si>
@@ -45,23 +46,41 @@
     <t>F1</t>
   </si>
   <si>
-    <t>not same method best for all parameters</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>Grobid best</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>best ident</t>
+  </si>
+  <si>
+    <t>grobid best</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,15 +114,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -996,6 +1073,240 @@
           </cell>
           <cell r="M23">
             <v>13.88</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3">
+            <v>87.63</v>
+          </cell>
+          <cell r="F3">
+            <v>85</v>
+          </cell>
+          <cell r="G3">
+            <v>85</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>69.66</v>
+          </cell>
+          <cell r="F4">
+            <v>67.39</v>
+          </cell>
+          <cell r="G4">
+            <v>67.39</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5" t="str">
+            <v>NAN</v>
+          </cell>
+          <cell r="F5">
+            <v>0</v>
+          </cell>
+          <cell r="G5">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="E6">
+            <v>82.73</v>
+          </cell>
+          <cell r="F6">
+            <v>63.94</v>
+          </cell>
+          <cell r="G6">
+            <v>61.94</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>84.32</v>
+          </cell>
+          <cell r="F7">
+            <v>88.4</v>
+          </cell>
+          <cell r="G7">
+            <v>83.84</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8">
+            <v>90.32</v>
+          </cell>
+          <cell r="F8">
+            <v>61.96</v>
+          </cell>
+          <cell r="G8">
+            <v>63.69</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>85.59</v>
+          </cell>
+          <cell r="F9">
+            <v>58.33</v>
+          </cell>
+          <cell r="G9">
+            <v>60.07</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>88.16</v>
+          </cell>
+          <cell r="F10">
+            <v>79.040000000000006</v>
+          </cell>
+          <cell r="G10">
+            <v>78.680000000000007</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>65.290000000000006</v>
+          </cell>
+          <cell r="F11">
+            <v>66.89</v>
+          </cell>
+          <cell r="G11">
+            <v>61.56</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="E12">
+            <v>62.5</v>
+          </cell>
+          <cell r="F12">
+            <v>26.32</v>
+          </cell>
+          <cell r="G12">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>60</v>
+          </cell>
+          <cell r="F13">
+            <v>100</v>
+          </cell>
+          <cell r="G13">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="E14">
+            <v>50</v>
+          </cell>
+          <cell r="F14">
+            <v>100</v>
+          </cell>
+          <cell r="G14">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="E15">
+            <v>75</v>
+          </cell>
+          <cell r="F15">
+            <v>75</v>
+          </cell>
+          <cell r="G15">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="E16">
+            <v>75</v>
+          </cell>
+          <cell r="F16">
+            <v>75</v>
+          </cell>
+          <cell r="G16">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="E17">
+            <v>83.33</v>
+          </cell>
+          <cell r="F17">
+            <v>31.25</v>
+          </cell>
+          <cell r="G17">
+            <v>29.41</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="E18">
+            <v>100</v>
+          </cell>
+          <cell r="F18">
+            <v>100</v>
+          </cell>
+          <cell r="G18">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="E19">
+            <v>83.45</v>
+          </cell>
+          <cell r="F19">
+            <v>83.95</v>
+          </cell>
+          <cell r="G19">
+            <v>81.75</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="E20">
+            <v>95.45</v>
+          </cell>
+          <cell r="F20">
+            <v>84.14</v>
+          </cell>
+          <cell r="G20">
+            <v>86.99</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="E21">
+            <v>63.03</v>
+          </cell>
+          <cell r="F21">
+            <v>48.11</v>
+          </cell>
+          <cell r="G21">
+            <v>49.02</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="E22">
+            <v>92.24</v>
+          </cell>
+          <cell r="F22">
+            <v>91.57</v>
+          </cell>
+          <cell r="G22">
+            <v>89.11</v>
           </cell>
         </row>
       </sheetData>
@@ -1301,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:G23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1312,768 +1623,1680 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="259" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="269" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="str">
         <f>'[1]Tabelle 1'!A2</f>
         <v>Id</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
+      <c r="W2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="str">
         <f>'[1]Tabelle 1'!A3</f>
         <v>Title</v>
       </c>
-      <c r="B2" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B3=C2,"Cermine",IF('[1]Tabelle 1'!C3=C2,"Grobid",IF('[1]Tabelle 1'!D3=C2,"ParsCit",IF('[1]Tabelle 1'!E3=C2,"PDFX","none"))))</f>
+      <c r="B3" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B3=C3,"Cermine",IF('[1]Tabelle 1'!C3=C3,"Grobid",IF('[1]Tabelle 1'!D3=C3,"ParsCit",IF('[1]Tabelle 1'!E3=C3,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" s="2">
         <f>MAX('[1]Tabelle 1'!B3:E3)</f>
         <v>94.79</v>
       </c>
-      <c r="D2" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F3=E2,"Cermine",IF('[1]Tabelle 1'!G3=E2,"Grobid",IF('[1]Tabelle 1'!H3=E2,"ParsCit",IF('[1]Tabelle 1'!I3=E2,"PDFX","none"))))</f>
+      <c r="D3" s="2" t="b">
+        <f t="shared" ref="D3:D22" si="0">B3="Grobid"</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <f>'[2]Tabelle 1'!E3</f>
+        <v>87.63</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F22" si="1">C3-E3</f>
+        <v>7.1600000000000108</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F3=H3,"Cermine",IF('[1]Tabelle 1'!G3=H3,"Grobid",IF('[1]Tabelle 1'!H3=H3,"ParsCit",IF('[1]Tabelle 1'!I3=H3,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E2" s="3">
+      <c r="H3" s="2">
         <f>MAX('[1]Tabelle 1'!F3:I3)</f>
         <v>91</v>
       </c>
-      <c r="F2" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J3=G2,"Cermine",IF('[1]Tabelle 1'!K3=G2,"Grobid",IF('[1]Tabelle 1'!L3=G2,"ParsCit",IF('[1]Tabelle 1'!M3=G2,"PDFX","none"))))</f>
+      <c r="I3" s="2" t="b">
+        <f t="shared" ref="I3:I22" si="2">G3="Grobid"</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <f>'[2]Tabelle 1'!F3</f>
+        <v>85</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K22" si="3">H3-J3</f>
+        <v>6</v>
+      </c>
+      <c r="L3" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J3=M3,"Cermine",IF('[1]Tabelle 1'!K3=M3,"Grobid",IF('[1]Tabelle 1'!L3=M3,"ParsCit",IF('[1]Tabelle 1'!M3=M3,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="G2" s="3">
+      <c r="M3" s="2">
         <f>MAX('[1]Tabelle 1'!J3:M3)</f>
         <v>91</v>
       </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f>COUNTIF(B$2:B$21,$I2)</f>
+      <c r="N3" s="2" t="b">
+        <f>L3="Grobid"</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <f>'[2]Tabelle 1'!G3</f>
+        <v>85</v>
+      </c>
+      <c r="P3" s="2">
+        <f>M3-O3</f>
+        <v>6</v>
+      </c>
+      <c r="Q3" s="2" t="b">
+        <f>AND(EXACT($B3,$G3),EXACT($G3,$L3))</f>
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>COUNTIF(B$3:B$22,$S3)</f>
         <v>3</v>
       </c>
-      <c r="K2">
-        <f>COUNTIF(D$2:D$21,$I2)</f>
+      <c r="U3">
+        <f>COUNTIF(G$3:G$22,$S3)</f>
         <v>9</v>
       </c>
-      <c r="L2">
-        <f>COUNTIF(F$2:F$21,$I2)</f>
+      <c r="V3">
+        <f>COUNTIF(L$3:L$22,$S3)</f>
         <v>4</v>
       </c>
-      <c r="M2">
-        <f>SUM(J2:L2)</f>
+      <c r="W3">
+        <f>SUM(T3:V3)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="str">
         <f>'[1]Tabelle 1'!A4</f>
         <v>Abstract</v>
       </c>
-      <c r="B3" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B4=C3,"Cermine",IF('[1]Tabelle 1'!C4=C3,"Grobid",IF('[1]Tabelle 1'!D4=C3,"ParsCit",IF('[1]Tabelle 1'!E4=C3,"PDFX","none"))))</f>
+      <c r="B4" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B4=C4,"Cermine",IF('[1]Tabelle 1'!C4=C4,"Grobid",IF('[1]Tabelle 1'!D4=C4,"ParsCit",IF('[1]Tabelle 1'!E4=C4,"PDFX","none"))))</f>
         <v>PDFX</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="2">
         <f>MAX('[1]Tabelle 1'!B4:E4)</f>
         <v>83.1</v>
       </c>
-      <c r="D3" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F4=E3,"Cermine",IF('[1]Tabelle 1'!G4=E3,"Grobid",IF('[1]Tabelle 1'!H4=E3,"ParsCit",IF('[1]Tabelle 1'!I4=E3,"PDFX","none"))))</f>
+      <c r="D4" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <f>'[2]Tabelle 1'!E4</f>
+        <v>69.66</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>13.439999999999998</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F4=H4,"Cermine",IF('[1]Tabelle 1'!G4=H4,"Grobid",IF('[1]Tabelle 1'!H4=H4,"ParsCit",IF('[1]Tabelle 1'!I4=H4,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E3" s="3">
+      <c r="H4" s="2">
         <f>MAX('[1]Tabelle 1'!F4:I4)</f>
         <v>69.569999999999993</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J4=G3,"Cermine",IF('[1]Tabelle 1'!K4=G3,"Grobid",IF('[1]Tabelle 1'!L4=G3,"ParsCit",IF('[1]Tabelle 1'!M4=G3,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="I4" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <f>'[2]Tabelle 1'!F4</f>
+        <v>67.39</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1799999999999926</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J4=M4,"Cermine",IF('[1]Tabelle 1'!K4=M4,"Grobid",IF('[1]Tabelle 1'!L4=M4,"ParsCit",IF('[1]Tabelle 1'!M4=M4,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M4" s="2">
         <f>MAX('[1]Tabelle 1'!J4:M4)</f>
         <v>67.39</v>
       </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J5" si="0">COUNTIF(B$2:B$21,$I3)</f>
+      <c r="N4" s="2" t="b">
+        <f t="shared" ref="N4:N24" si="4">L4="Grobid"</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <f>'[2]Tabelle 1'!G4</f>
+        <v>67.39</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P24" si="5">M4-O4</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="b">
+        <f t="shared" ref="Q4:Q24" si="6">AND(EXACT($B4,$G4),EXACT($G4,$L4))</f>
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <f>COUNTIF(B$3:B$22,$S4)</f>
         <v>14</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K5" si="1">COUNTIF(D$2:D$21,$I3)</f>
+      <c r="U4">
+        <f>COUNTIF(G$3:G$22,$S4)</f>
         <v>11</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L5" si="2">COUNTIF(F$2:F$21,$I3)</f>
+      <c r="V4">
+        <f>COUNTIF(L$3:L$22,$S4)</f>
         <v>15</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M5" si="3">SUM(J3:L3)</f>
+      <c r="W4">
+        <f t="shared" ref="W4:W6" si="7">SUM(T4:V4)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="str">
         <f>'[1]Tabelle 1'!A5</f>
         <v>Abstract (german)</v>
       </c>
-      <c r="B4" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B5=C4,"Cermine",IF('[1]Tabelle 1'!C5=C4,"Grobid",IF('[1]Tabelle 1'!D5=C4,"ParsCit",IF('[1]Tabelle 1'!E5=C4,"PDFX","none"))))</f>
+      <c r="B5" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B5=C5,"Cermine",IF('[1]Tabelle 1'!C5=C5,"Grobid",IF('[1]Tabelle 1'!D5=C5,"ParsCit",IF('[1]Tabelle 1'!E5=C5,"PDFX","none"))))</f>
         <v>none</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="2">
         <f>MAX('[1]Tabelle 1'!B5:E5)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F5=E4,"Cermine",IF('[1]Tabelle 1'!G5=E4,"Grobid",IF('[1]Tabelle 1'!H5=E4,"ParsCit",IF('[1]Tabelle 1'!I5=E4,"PDFX","none"))))</f>
+      <c r="D5" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>'[2]Tabelle 1'!E5</f>
+        <v>NAN</v>
+      </c>
+      <c r="F5" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F5=H5,"Cermine",IF('[1]Tabelle 1'!G5=H5,"Grobid",IF('[1]Tabelle 1'!H5=H5,"ParsCit",IF('[1]Tabelle 1'!I5=H5,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E4" s="3">
+      <c r="H5" s="2">
         <f>MAX('[1]Tabelle 1'!F5:I5)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J5=G4,"Cermine",IF('[1]Tabelle 1'!K5=G4,"Grobid",IF('[1]Tabelle 1'!L5=G4,"ParsCit",IF('[1]Tabelle 1'!M5=G4,"PDFX","none"))))</f>
+      <c r="I5" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f>'[2]Tabelle 1'!F5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J5=M5,"Cermine",IF('[1]Tabelle 1'!K5=M5,"Grobid",IF('[1]Tabelle 1'!L5=M5,"ParsCit",IF('[1]Tabelle 1'!M5=M5,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="G4" s="3">
+      <c r="M5" s="2">
         <f>MAX('[1]Tabelle 1'!J5:M5)</f>
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N5" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <f>'[2]Tabelle 1'!G5</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
         <v>2</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
+      <c r="T5">
+        <f>COUNTIF(B$3:B$22,$S5)</f>
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <f>COUNTIF(G$3:G$22,$S5)</f>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f>COUNTIF(L$3:L$22,$S5)</f>
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="str">
         <f>'[1]Tabelle 1'!A6</f>
         <v>Keywords</v>
       </c>
-      <c r="B5" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B6=C5,"Cermine",IF('[1]Tabelle 1'!C6=C5,"Grobid",IF('[1]Tabelle 1'!D6=C5,"ParsCit",IF('[1]Tabelle 1'!E6=C5,"PDFX","none"))))</f>
+      <c r="B6" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B6=C6,"Cermine",IF('[1]Tabelle 1'!C6=C6,"Grobid",IF('[1]Tabelle 1'!D6=C6,"ParsCit",IF('[1]Tabelle 1'!E6=C6,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="2">
         <f>MAX('[1]Tabelle 1'!B6:E6)</f>
         <v>84.67</v>
       </c>
-      <c r="D5" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F6=E5,"Cermine",IF('[1]Tabelle 1'!G6=E5,"Grobid",IF('[1]Tabelle 1'!H6=E5,"ParsCit",IF('[1]Tabelle 1'!I6=E5,"PDFX","none"))))</f>
+      <c r="D6" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <f>'[2]Tabelle 1'!E6</f>
+        <v>82.73</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9399999999999977</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F6=H6,"Cermine",IF('[1]Tabelle 1'!G6=H6,"Grobid",IF('[1]Tabelle 1'!H6=H6,"ParsCit",IF('[1]Tabelle 1'!I6=H6,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E5" s="3">
+      <c r="H6" s="2">
         <f>MAX('[1]Tabelle 1'!F6:I6)</f>
         <v>67.959999999999994</v>
       </c>
-      <c r="F5" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J6=G5,"Cermine",IF('[1]Tabelle 1'!K6=G5,"Grobid",IF('[1]Tabelle 1'!L6=G5,"ParsCit",IF('[1]Tabelle 1'!M6=G5,"PDFX","none"))))</f>
+      <c r="I6" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <f>'[2]Tabelle 1'!F6</f>
+        <v>63.94</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>4.019999999999996</v>
+      </c>
+      <c r="L6" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J6=M6,"Cermine",IF('[1]Tabelle 1'!K6=M6,"Grobid",IF('[1]Tabelle 1'!L6=M6,"ParsCit",IF('[1]Tabelle 1'!M6=M6,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="G5" s="3">
+      <c r="M6" s="2">
         <f>MAX('[1]Tabelle 1'!J6:M6)</f>
         <v>63.97</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N6" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <f>'[2]Tabelle 1'!G6</f>
+        <v>61.94</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0300000000000011</v>
+      </c>
+      <c r="Q6" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
         <v>3</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
+      <c r="T6">
+        <f>COUNTIF(B$3:B$22,$S6)</f>
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <f>COUNTIF(G$3:G$22,$S6)</f>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f>COUNTIF(L$3:L$22,$S6)</f>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="str">
         <f>'[1]Tabelle 1'!A7</f>
         <v>Authors</v>
       </c>
-      <c r="B6" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B7=C6,"Cermine",IF('[1]Tabelle 1'!C7=C6,"Grobid",IF('[1]Tabelle 1'!D7=C6,"ParsCit",IF('[1]Tabelle 1'!E7=C6,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B7" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B7=C7,"Cermine",IF('[1]Tabelle 1'!C7=C7,"Grobid",IF('[1]Tabelle 1'!D7=C7,"ParsCit",IF('[1]Tabelle 1'!E7=C7,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C7" s="2">
         <f>MAX('[1]Tabelle 1'!B7:E7)</f>
         <v>85.58</v>
       </c>
-      <c r="D6" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F7=E6,"Cermine",IF('[1]Tabelle 1'!G7=E6,"Grobid",IF('[1]Tabelle 1'!H7=E6,"ParsCit",IF('[1]Tabelle 1'!I7=E6,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D7" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <f>'[2]Tabelle 1'!E7</f>
+        <v>84.32</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2600000000000051</v>
+      </c>
+      <c r="G7" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F7=H7,"Cermine",IF('[1]Tabelle 1'!G7=H7,"Grobid",IF('[1]Tabelle 1'!H7=H7,"ParsCit",IF('[1]Tabelle 1'!I7=H7,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H7" s="2">
         <f>MAX('[1]Tabelle 1'!F7:I7)</f>
         <v>89.35</v>
       </c>
-      <c r="F6" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J7=G6,"Cermine",IF('[1]Tabelle 1'!K7=G6,"Grobid",IF('[1]Tabelle 1'!L7=G6,"ParsCit",IF('[1]Tabelle 1'!M7=G6,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="I7" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <f>'[2]Tabelle 1'!F7</f>
+        <v>88.4</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.94999999999998863</v>
+      </c>
+      <c r="L7" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J7=M7,"Cermine",IF('[1]Tabelle 1'!K7=M7,"Grobid",IF('[1]Tabelle 1'!L7=M7,"ParsCit",IF('[1]Tabelle 1'!M7=M7,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M7" s="2">
         <f>MAX('[1]Tabelle 1'!J7:M7)</f>
         <v>84.87</v>
       </c>
+      <c r="N7" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <f>'[2]Tabelle 1'!G7</f>
+        <v>83.84</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0300000000000011</v>
+      </c>
+      <c r="Q7" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="str">
         <f>'[1]Tabelle 1'!A8</f>
         <v>Emails</v>
       </c>
-      <c r="B7" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B8=C7,"Cermine",IF('[1]Tabelle 1'!C8=C7,"Grobid",IF('[1]Tabelle 1'!D8=C7,"ParsCit",IF('[1]Tabelle 1'!E8=C7,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B8" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B8=C8,"Cermine",IF('[1]Tabelle 1'!C8=C8,"Grobid",IF('[1]Tabelle 1'!D8=C8,"ParsCit",IF('[1]Tabelle 1'!E8=C8,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C8" s="2">
         <f>MAX('[1]Tabelle 1'!B8:E8)</f>
         <v>90.32</v>
       </c>
-      <c r="D7" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F8=E7,"Cermine",IF('[1]Tabelle 1'!G8=E7,"Grobid",IF('[1]Tabelle 1'!H8=E7,"ParsCit",IF('[1]Tabelle 1'!I8=E7,"PDFX","none"))))</f>
+      <c r="D8" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <f>'[2]Tabelle 1'!E8</f>
+        <v>90.32</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F8=H8,"Cermine",IF('[1]Tabelle 1'!G8=H8,"Grobid",IF('[1]Tabelle 1'!H8=H8,"ParsCit",IF('[1]Tabelle 1'!I8=H8,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E7" s="3">
+      <c r="H8" s="2">
         <f>MAX('[1]Tabelle 1'!F8:I8)</f>
         <v>70.650000000000006</v>
       </c>
-      <c r="F7" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J8=G7,"Cermine",IF('[1]Tabelle 1'!K8=G7,"Grobid",IF('[1]Tabelle 1'!L8=G7,"ParsCit",IF('[1]Tabelle 1'!M8=G7,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="I8" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f>'[2]Tabelle 1'!F8</f>
+        <v>61.96</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>8.6900000000000048</v>
+      </c>
+      <c r="L8" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J8=M8,"Cermine",IF('[1]Tabelle 1'!K8=M8,"Grobid",IF('[1]Tabelle 1'!L8=M8,"ParsCit",IF('[1]Tabelle 1'!M8=M8,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M8" s="2">
         <f>MAX('[1]Tabelle 1'!J8:M8)</f>
         <v>63.69</v>
       </c>
+      <c r="N8" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <f>'[2]Tabelle 1'!G8</f>
+        <v>63.69</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="str">
         <f>'[1]Tabelle 1'!A9</f>
         <v>Author-Emails</v>
       </c>
-      <c r="B8" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B9=C8,"Cermine",IF('[1]Tabelle 1'!C9=C8,"Grobid",IF('[1]Tabelle 1'!D9=C8,"ParsCit",IF('[1]Tabelle 1'!E9=C8,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B9" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B9=C9,"Cermine",IF('[1]Tabelle 1'!C9=C9,"Grobid",IF('[1]Tabelle 1'!D9=C9,"ParsCit",IF('[1]Tabelle 1'!E9=C9,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C9" s="2">
         <f>MAX('[1]Tabelle 1'!B9:E9)</f>
         <v>85.59</v>
       </c>
-      <c r="D8" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F9=E8,"Cermine",IF('[1]Tabelle 1'!G9=E8,"Grobid",IF('[1]Tabelle 1'!H9=E8,"ParsCit",IF('[1]Tabelle 1'!I9=E8,"PDFX","none"))))</f>
+      <c r="D9" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <f>'[2]Tabelle 1'!E9</f>
+        <v>85.59</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F9=H9,"Cermine",IF('[1]Tabelle 1'!G9=H9,"Grobid",IF('[1]Tabelle 1'!H9=H9,"ParsCit",IF('[1]Tabelle 1'!I9=H9,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E8" s="3">
+      <c r="H9" s="2">
         <f>MAX('[1]Tabelle 1'!F9:I9)</f>
         <v>66.67</v>
       </c>
-      <c r="F8" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J9=G8,"Cermine",IF('[1]Tabelle 1'!K9=G8,"Grobid",IF('[1]Tabelle 1'!L9=G8,"ParsCit",IF('[1]Tabelle 1'!M9=G8,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="I9" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <f>'[2]Tabelle 1'!F9</f>
+        <v>58.33</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>8.3400000000000034</v>
+      </c>
+      <c r="L9" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J9=M9,"Cermine",IF('[1]Tabelle 1'!K9=M9,"Grobid",IF('[1]Tabelle 1'!L9=M9,"ParsCit",IF('[1]Tabelle 1'!M9=M9,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M9" s="2">
         <f>MAX('[1]Tabelle 1'!J9:M9)</f>
         <v>60.07</v>
       </c>
+      <c r="N9" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="2">
+        <f>'[2]Tabelle 1'!G9</f>
+        <v>60.07</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="str">
         <f>'[1]Tabelle 1'!A10</f>
         <v>Affiliations</v>
       </c>
-      <c r="B9" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B10=C9,"Cermine",IF('[1]Tabelle 1'!C10=C9,"Grobid",IF('[1]Tabelle 1'!D10=C9,"ParsCit",IF('[1]Tabelle 1'!E10=C9,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B10" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B10=C10,"Cermine",IF('[1]Tabelle 1'!C10=C10,"Grobid",IF('[1]Tabelle 1'!D10=C10,"ParsCit",IF('[1]Tabelle 1'!E10=C10,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C10" s="2">
         <f>MAX('[1]Tabelle 1'!B10:E10)</f>
         <v>89.29</v>
       </c>
-      <c r="D9" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F10=E9,"Cermine",IF('[1]Tabelle 1'!G10=E9,"Grobid",IF('[1]Tabelle 1'!H10=E9,"ParsCit",IF('[1]Tabelle 1'!I10=E9,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="D10" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <f>'[2]Tabelle 1'!E10</f>
+        <v>88.16</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1300000000000097</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F10=H10,"Cermine",IF('[1]Tabelle 1'!G10=H10,"Grobid",IF('[1]Tabelle 1'!H10=H10,"ParsCit",IF('[1]Tabelle 1'!I10=H10,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H10" s="2">
         <f>MAX('[1]Tabelle 1'!F10:I10)</f>
         <v>82.68</v>
       </c>
-      <c r="F9" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J10=G9,"Cermine",IF('[1]Tabelle 1'!K10=G9,"Grobid",IF('[1]Tabelle 1'!L10=G9,"ParsCit",IF('[1]Tabelle 1'!M10=G9,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="I10" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <f>'[2]Tabelle 1'!F10</f>
+        <v>79.040000000000006</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>3.6400000000000006</v>
+      </c>
+      <c r="L10" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J10=M10,"Cermine",IF('[1]Tabelle 1'!K10=M10,"Grobid",IF('[1]Tabelle 1'!L10=M10,"ParsCit",IF('[1]Tabelle 1'!M10=M10,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M10" s="2">
         <f>MAX('[1]Tabelle 1'!J10:M10)</f>
         <v>82.4</v>
       </c>
+      <c r="N10" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
+        <f>'[2]Tabelle 1'!G10</f>
+        <v>78.680000000000007</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="5"/>
+        <v>3.7199999999999989</v>
+      </c>
+      <c r="Q10" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="str">
         <f>'[1]Tabelle 1'!A11</f>
         <v>Author-Affiliations</v>
       </c>
-      <c r="B10" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B11=C10,"Cermine",IF('[1]Tabelle 1'!C11=C10,"Grobid",IF('[1]Tabelle 1'!D11=C10,"ParsCit",IF('[1]Tabelle 1'!E11=C10,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B11" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B11=C11,"Cermine",IF('[1]Tabelle 1'!C11=C11,"Grobid",IF('[1]Tabelle 1'!D11=C11,"ParsCit",IF('[1]Tabelle 1'!E11=C11,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C11" s="2">
         <f>MAX('[1]Tabelle 1'!B11:E11)</f>
         <v>65.89</v>
       </c>
-      <c r="D10" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F11=E10,"Cermine",IF('[1]Tabelle 1'!G11=E10,"Grobid",IF('[1]Tabelle 1'!H11=E10,"ParsCit",IF('[1]Tabelle 1'!I11=E10,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D11" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <f>'[2]Tabelle 1'!E11</f>
+        <v>65.290000000000006</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.59999999999999432</v>
+      </c>
+      <c r="G11" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F11=H11,"Cermine",IF('[1]Tabelle 1'!G11=H11,"Grobid",IF('[1]Tabelle 1'!H11=H11,"ParsCit",IF('[1]Tabelle 1'!I11=H11,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H11" s="2">
         <f>MAX('[1]Tabelle 1'!F11:I11)</f>
         <v>69.599999999999994</v>
       </c>
-      <c r="F10" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J11=G10,"Cermine",IF('[1]Tabelle 1'!K11=G10,"Grobid",IF('[1]Tabelle 1'!L11=G10,"ParsCit",IF('[1]Tabelle 1'!M11=G10,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="I11" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <f>'[2]Tabelle 1'!F11</f>
+        <v>66.89</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>2.7099999999999937</v>
+      </c>
+      <c r="L11" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J11=M11,"Cermine",IF('[1]Tabelle 1'!K11=M11,"Grobid",IF('[1]Tabelle 1'!L11=M11,"ParsCit",IF('[1]Tabelle 1'!M11=M11,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M11" s="2">
         <f>MAX('[1]Tabelle 1'!J11:M11)</f>
         <v>64.02</v>
       </c>
+      <c r="N11" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="2">
+        <f>'[2]Tabelle 1'!G11</f>
+        <v>61.56</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="5"/>
+        <v>2.4599999999999937</v>
+      </c>
+      <c r="Q11" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="str">
         <f>'[1]Tabelle 1'!A12</f>
         <v>Source</v>
       </c>
-      <c r="B11" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B12=C11,"Cermine",IF('[1]Tabelle 1'!C12=C11,"Grobid",IF('[1]Tabelle 1'!D12=C11,"ParsCit",IF('[1]Tabelle 1'!E12=C11,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B12" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B12=C12,"Cermine",IF('[1]Tabelle 1'!C12=C12,"Grobid",IF('[1]Tabelle 1'!D12=C12,"ParsCit",IF('[1]Tabelle 1'!E12=C12,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C12" s="2">
         <f>MAX('[1]Tabelle 1'!B12:E12)</f>
         <v>66.67</v>
       </c>
-      <c r="D11" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F12=E11,"Cermine",IF('[1]Tabelle 1'!G12=E11,"Grobid",IF('[1]Tabelle 1'!H12=E11,"ParsCit",IF('[1]Tabelle 1'!I12=E11,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D12" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <f>'[2]Tabelle 1'!E12</f>
+        <v>62.5</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1700000000000017</v>
+      </c>
+      <c r="G12" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F12=H12,"Cermine",IF('[1]Tabelle 1'!G12=H12,"Grobid",IF('[1]Tabelle 1'!H12=H12,"ParsCit",IF('[1]Tabelle 1'!I12=H12,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H12" s="2">
         <f>MAX('[1]Tabelle 1'!F12:I12)</f>
         <v>21.05</v>
       </c>
-      <c r="F11" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J12=G11,"Cermine",IF('[1]Tabelle 1'!K12=G11,"Grobid",IF('[1]Tabelle 1'!L12=G11,"ParsCit",IF('[1]Tabelle 1'!M12=G11,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="I12" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <f>'[2]Tabelle 1'!F12</f>
+        <v>26.32</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>-5.27</v>
+      </c>
+      <c r="L12" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J12=M12,"Cermine",IF('[1]Tabelle 1'!K12=M12,"Grobid",IF('[1]Tabelle 1'!L12=M12,"ParsCit",IF('[1]Tabelle 1'!M12=M12,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M12" s="2">
         <f>MAX('[1]Tabelle 1'!J12:M12)</f>
         <v>20</v>
       </c>
+      <c r="N12" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="2">
+        <f>'[2]Tabelle 1'!G12</f>
+        <v>25</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="Q12" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="str">
         <f>'[1]Tabelle 1'!A13</f>
         <v>Volume</v>
       </c>
-      <c r="B12" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B13=C12,"Cermine",IF('[1]Tabelle 1'!C13=C12,"Grobid",IF('[1]Tabelle 1'!D13=C12,"ParsCit",IF('[1]Tabelle 1'!E13=C12,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B13" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B13=C13,"Cermine",IF('[1]Tabelle 1'!C13=C13,"Grobid",IF('[1]Tabelle 1'!D13=C13,"ParsCit",IF('[1]Tabelle 1'!E13=C13,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C13" s="2">
         <f>MAX('[1]Tabelle 1'!B13:E13)</f>
         <v>100</v>
       </c>
-      <c r="D12" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F13=E12,"Cermine",IF('[1]Tabelle 1'!G13=E12,"Grobid",IF('[1]Tabelle 1'!H13=E12,"ParsCit",IF('[1]Tabelle 1'!I13=E12,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="D13" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <f>'[2]Tabelle 1'!E13</f>
+        <v>60</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G13" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F13=H13,"Cermine",IF('[1]Tabelle 1'!G13=H13,"Grobid",IF('[1]Tabelle 1'!H13=H13,"ParsCit",IF('[1]Tabelle 1'!I13=H13,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H13" s="2">
         <f>MAX('[1]Tabelle 1'!F13:I13)</f>
         <v>100</v>
       </c>
-      <c r="F12" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J13=G12,"Cermine",IF('[1]Tabelle 1'!K13=G12,"Grobid",IF('[1]Tabelle 1'!L13=G12,"ParsCit",IF('[1]Tabelle 1'!M13=G12,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="I13" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <f>'[2]Tabelle 1'!F13</f>
+        <v>100</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J13=M13,"Cermine",IF('[1]Tabelle 1'!K13=M13,"Grobid",IF('[1]Tabelle 1'!L13=M13,"ParsCit",IF('[1]Tabelle 1'!M13=M13,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M13" s="2">
         <f>MAX('[1]Tabelle 1'!J13:M13)</f>
         <v>100</v>
       </c>
+      <c r="N13" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <f>'[2]Tabelle 1'!G13</f>
+        <v>60</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="Q13" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="str">
         <f>'[1]Tabelle 1'!A14</f>
         <v>Issue</v>
       </c>
-      <c r="B13" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B14=C13,"Cermine",IF('[1]Tabelle 1'!C14=C13,"Grobid",IF('[1]Tabelle 1'!D14=C13,"ParsCit",IF('[1]Tabelle 1'!E14=C13,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B14" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B14=C14,"Cermine",IF('[1]Tabelle 1'!C14=C14,"Grobid",IF('[1]Tabelle 1'!D14=C14,"ParsCit",IF('[1]Tabelle 1'!E14=C14,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C14" s="2">
         <f>MAX('[1]Tabelle 1'!B14:E14)</f>
         <v>100</v>
       </c>
-      <c r="D13" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F14=E13,"Cermine",IF('[1]Tabelle 1'!G14=E13,"Grobid",IF('[1]Tabelle 1'!H14=E13,"ParsCit",IF('[1]Tabelle 1'!I14=E13,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="D14" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <f>'[2]Tabelle 1'!E14</f>
+        <v>50</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="G14" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F14=H14,"Cermine",IF('[1]Tabelle 1'!G14=H14,"Grobid",IF('[1]Tabelle 1'!H14=H14,"ParsCit",IF('[1]Tabelle 1'!I14=H14,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H14" s="2">
         <f>MAX('[1]Tabelle 1'!F14:I14)</f>
         <v>100</v>
       </c>
-      <c r="F13" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J14=G13,"Cermine",IF('[1]Tabelle 1'!K14=G13,"Grobid",IF('[1]Tabelle 1'!L14=G13,"ParsCit",IF('[1]Tabelle 1'!M14=G13,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="I14" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <f>'[2]Tabelle 1'!F14</f>
+        <v>100</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J14=M14,"Cermine",IF('[1]Tabelle 1'!K14=M14,"Grobid",IF('[1]Tabelle 1'!L14=M14,"ParsCit",IF('[1]Tabelle 1'!M14=M14,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M14" s="2">
         <f>MAX('[1]Tabelle 1'!J14:M14)</f>
         <v>100</v>
       </c>
+      <c r="N14" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
+        <f>'[2]Tabelle 1'!G14</f>
+        <v>50</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="Q14" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="str">
         <f>'[1]Tabelle 1'!A15</f>
         <v>Page from</v>
       </c>
-      <c r="B14" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B15=C14,"Cermine",IF('[1]Tabelle 1'!C15=C14,"Grobid",IF('[1]Tabelle 1'!D15=C14,"ParsCit",IF('[1]Tabelle 1'!E15=C14,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B15" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B15=C15,"Cermine",IF('[1]Tabelle 1'!C15=C15,"Grobid",IF('[1]Tabelle 1'!D15=C15,"ParsCit",IF('[1]Tabelle 1'!E15=C15,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C15" s="2">
         <f>MAX('[1]Tabelle 1'!B15:E15)</f>
         <v>100</v>
       </c>
-      <c r="D14" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F15=E14,"Cermine",IF('[1]Tabelle 1'!G15=E14,"Grobid",IF('[1]Tabelle 1'!H15=E14,"ParsCit",IF('[1]Tabelle 1'!I15=E14,"PDFX","none"))))</f>
+      <c r="D15" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <f>'[2]Tabelle 1'!E15</f>
+        <v>75</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G15" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F15=H15,"Cermine",IF('[1]Tabelle 1'!G15=H15,"Grobid",IF('[1]Tabelle 1'!H15=H15,"ParsCit",IF('[1]Tabelle 1'!I15=H15,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E14" s="3">
+      <c r="H15" s="2">
         <f>MAX('[1]Tabelle 1'!F15:I15)</f>
         <v>100</v>
       </c>
-      <c r="F14" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J15=G14,"Cermine",IF('[1]Tabelle 1'!K15=G14,"Grobid",IF('[1]Tabelle 1'!L15=G14,"ParsCit",IF('[1]Tabelle 1'!M15=G14,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="I15" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f>'[2]Tabelle 1'!F15</f>
+        <v>75</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L15" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J15=M15,"Cermine",IF('[1]Tabelle 1'!K15=M15,"Grobid",IF('[1]Tabelle 1'!L15=M15,"ParsCit",IF('[1]Tabelle 1'!M15=M15,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M15" s="2">
         <f>MAX('[1]Tabelle 1'!J15:M15)</f>
         <v>50</v>
       </c>
+      <c r="N15" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <f>'[2]Tabelle 1'!G15</f>
+        <v>60</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="Q15" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="str">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="str">
         <f>'[1]Tabelle 1'!A16</f>
         <v>Page to</v>
       </c>
-      <c r="B15" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B16=C15,"Cermine",IF('[1]Tabelle 1'!C16=C15,"Grobid",IF('[1]Tabelle 1'!D16=C15,"ParsCit",IF('[1]Tabelle 1'!E16=C15,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B16" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B16=C16,"Cermine",IF('[1]Tabelle 1'!C16=C16,"Grobid",IF('[1]Tabelle 1'!D16=C16,"ParsCit",IF('[1]Tabelle 1'!E16=C16,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C16" s="2">
         <f>MAX('[1]Tabelle 1'!B16:E16)</f>
         <v>100</v>
       </c>
-      <c r="D15" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F16=E15,"Cermine",IF('[1]Tabelle 1'!G16=E15,"Grobid",IF('[1]Tabelle 1'!H16=E15,"ParsCit",IF('[1]Tabelle 1'!I16=E15,"PDFX","none"))))</f>
+      <c r="D16" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <f>'[2]Tabelle 1'!E16</f>
+        <v>75</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G16" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F16=H16,"Cermine",IF('[1]Tabelle 1'!G16=H16,"Grobid",IF('[1]Tabelle 1'!H16=H16,"ParsCit",IF('[1]Tabelle 1'!I16=H16,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E15" s="3">
+      <c r="H16" s="2">
         <f>MAX('[1]Tabelle 1'!F16:I16)</f>
         <v>100</v>
       </c>
-      <c r="F15" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J16=G15,"Cermine",IF('[1]Tabelle 1'!K16=G15,"Grobid",IF('[1]Tabelle 1'!L16=G15,"ParsCit",IF('[1]Tabelle 1'!M16=G15,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="I16" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f>'[2]Tabelle 1'!F16</f>
+        <v>75</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L16" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J16=M16,"Cermine",IF('[1]Tabelle 1'!K16=M16,"Grobid",IF('[1]Tabelle 1'!L16=M16,"ParsCit",IF('[1]Tabelle 1'!M16=M16,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M16" s="2">
         <f>MAX('[1]Tabelle 1'!J16:M16)</f>
         <v>50</v>
       </c>
+      <c r="N16" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="2">
+        <f>'[2]Tabelle 1'!G16</f>
+        <v>60</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="Q16" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="str">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="str">
         <f>'[1]Tabelle 1'!A17</f>
         <v>Year</v>
       </c>
-      <c r="B16" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B17=C16,"Cermine",IF('[1]Tabelle 1'!C17=C16,"Grobid",IF('[1]Tabelle 1'!D17=C16,"ParsCit",IF('[1]Tabelle 1'!E17=C16,"PDFX","none"))))</f>
+      <c r="B17" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B17=C17,"Cermine",IF('[1]Tabelle 1'!C17=C17,"Grobid",IF('[1]Tabelle 1'!D17=C17,"ParsCit",IF('[1]Tabelle 1'!E17=C17,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C17" s="2">
         <f>MAX('[1]Tabelle 1'!B17:E17)</f>
         <v>48.84</v>
       </c>
-      <c r="D16" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F17=E16,"Cermine",IF('[1]Tabelle 1'!G17=E16,"Grobid",IF('[1]Tabelle 1'!H17=E16,"ParsCit",IF('[1]Tabelle 1'!I17=E16,"PDFX","none"))))</f>
+      <c r="D17" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <f>'[2]Tabelle 1'!E17</f>
+        <v>83.33</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>-34.489999999999995</v>
+      </c>
+      <c r="G17" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F17=H17,"Cermine",IF('[1]Tabelle 1'!G17=H17,"Grobid",IF('[1]Tabelle 1'!H17=H17,"ParsCit",IF('[1]Tabelle 1'!I17=H17,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="E16" s="3">
+      <c r="H17" s="2">
         <f>MAX('[1]Tabelle 1'!F17:I17)</f>
         <v>65.63</v>
       </c>
-      <c r="F16" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J17=G16,"Cermine",IF('[1]Tabelle 1'!K17=G16,"Grobid",IF('[1]Tabelle 1'!L17=G16,"ParsCit",IF('[1]Tabelle 1'!M17=G16,"PDFX","none"))))</f>
+      <c r="I17" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f>'[2]Tabelle 1'!F17</f>
+        <v>31.25</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>34.379999999999995</v>
+      </c>
+      <c r="L17" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J17=M17,"Cermine",IF('[1]Tabelle 1'!K17=M17,"Grobid",IF('[1]Tabelle 1'!L17=M17,"ParsCit",IF('[1]Tabelle 1'!M17=M17,"PDFX","none"))))</f>
         <v>Cermine</v>
       </c>
-      <c r="G16" s="3">
+      <c r="M17" s="2">
         <f>MAX('[1]Tabelle 1'!J17:M17)</f>
         <v>46.67</v>
       </c>
+      <c r="N17" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <f>'[2]Tabelle 1'!G17</f>
+        <v>29.41</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="5"/>
+        <v>17.260000000000002</v>
+      </c>
+      <c r="Q17" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="str">
         <f>'[1]Tabelle 1'!A18</f>
         <v>Doi</v>
       </c>
-      <c r="B17" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B18=C17,"Cermine",IF('[1]Tabelle 1'!C18=C17,"Grobid",IF('[1]Tabelle 1'!D18=C17,"ParsCit",IF('[1]Tabelle 1'!E18=C17,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="B18" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B18=C18,"Cermine",IF('[1]Tabelle 1'!C18=C18,"Grobid",IF('[1]Tabelle 1'!D18=C18,"ParsCit",IF('[1]Tabelle 1'!E18=C18,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C18" s="2">
         <f>MAX('[1]Tabelle 1'!B18:E18)</f>
         <v>100</v>
       </c>
-      <c r="D17" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F18=E17,"Cermine",IF('[1]Tabelle 1'!G18=E17,"Grobid",IF('[1]Tabelle 1'!H18=E17,"ParsCit",IF('[1]Tabelle 1'!I18=E17,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="D18" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <f>'[2]Tabelle 1'!E18</f>
+        <v>100</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F18=H18,"Cermine",IF('[1]Tabelle 1'!G18=H18,"Grobid",IF('[1]Tabelle 1'!H18=H18,"ParsCit",IF('[1]Tabelle 1'!I18=H18,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H18" s="2">
         <f>MAX('[1]Tabelle 1'!F18:I18)</f>
         <v>100</v>
       </c>
-      <c r="F17" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J18=G17,"Cermine",IF('[1]Tabelle 1'!K18=G17,"Grobid",IF('[1]Tabelle 1'!L18=G17,"ParsCit",IF('[1]Tabelle 1'!M18=G17,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="I18" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <f>'[2]Tabelle 1'!F18</f>
+        <v>100</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J18=M18,"Cermine",IF('[1]Tabelle 1'!K18=M18,"Grobid",IF('[1]Tabelle 1'!L18=M18,"ParsCit",IF('[1]Tabelle 1'!M18=M18,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M18" s="2">
         <f>MAX('[1]Tabelle 1'!J18:M18)</f>
         <v>100</v>
       </c>
+      <c r="N18" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="2">
+        <f>'[2]Tabelle 1'!G18</f>
+        <v>100</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="str">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="str">
         <f>'[1]Tabelle 1'!A19</f>
         <v>Sections</v>
       </c>
-      <c r="B18" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B19=C18,"Cermine",IF('[1]Tabelle 1'!C19=C18,"Grobid",IF('[1]Tabelle 1'!D19=C18,"ParsCit",IF('[1]Tabelle 1'!E19=C18,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="B19" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B19=C19,"Cermine",IF('[1]Tabelle 1'!C19=C19,"Grobid",IF('[1]Tabelle 1'!D19=C19,"ParsCit",IF('[1]Tabelle 1'!E19=C19,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C19" s="2">
         <f>MAX('[1]Tabelle 1'!B19:E19)</f>
         <v>83.45</v>
       </c>
-      <c r="D18" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F19=E18,"Cermine",IF('[1]Tabelle 1'!G19=E18,"Grobid",IF('[1]Tabelle 1'!H19=E18,"ParsCit",IF('[1]Tabelle 1'!I19=E18,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D19" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <f>'[2]Tabelle 1'!E19</f>
+        <v>83.45</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F19=H19,"Cermine",IF('[1]Tabelle 1'!G19=H19,"Grobid",IF('[1]Tabelle 1'!H19=H19,"ParsCit",IF('[1]Tabelle 1'!I19=H19,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H19" s="2">
         <f>MAX('[1]Tabelle 1'!F19:I19)</f>
         <v>83.95</v>
       </c>
-      <c r="F18" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J19=G18,"Cermine",IF('[1]Tabelle 1'!K19=G18,"Grobid",IF('[1]Tabelle 1'!L19=G18,"ParsCit",IF('[1]Tabelle 1'!M19=G18,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="I19" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <f>'[2]Tabelle 1'!F19</f>
+        <v>83.95</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J19=M19,"Cermine",IF('[1]Tabelle 1'!K19=M19,"Grobid",IF('[1]Tabelle 1'!L19=M19,"ParsCit",IF('[1]Tabelle 1'!M19=M19,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M19" s="2">
         <f>MAX('[1]Tabelle 1'!J19:M19)</f>
         <v>81.75</v>
       </c>
+      <c r="N19" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="2">
+        <f>'[2]Tabelle 1'!G19</f>
+        <v>81.75</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="str">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="str">
         <f>'[1]Tabelle 1'!A20</f>
         <v>Section-Levels</v>
       </c>
-      <c r="B19" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B20=C19,"Cermine",IF('[1]Tabelle 1'!C20=C19,"Grobid",IF('[1]Tabelle 1'!D20=C19,"ParsCit",IF('[1]Tabelle 1'!E20=C19,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B20" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B20=C20,"Cermine",IF('[1]Tabelle 1'!C20=C20,"Grobid",IF('[1]Tabelle 1'!D20=C20,"ParsCit",IF('[1]Tabelle 1'!E20=C20,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C20" s="2">
         <f>MAX('[1]Tabelle 1'!B20:E20)</f>
         <v>95.45</v>
       </c>
-      <c r="D19" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F20=E19,"Cermine",IF('[1]Tabelle 1'!G20=E19,"Grobid",IF('[1]Tabelle 1'!H20=E19,"ParsCit",IF('[1]Tabelle 1'!I20=E19,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D20" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <f>'[2]Tabelle 1'!E20</f>
+        <v>95.45</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F20=H20,"Cermine",IF('[1]Tabelle 1'!G20=H20,"Grobid",IF('[1]Tabelle 1'!H20=H20,"ParsCit",IF('[1]Tabelle 1'!I20=H20,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H20" s="2">
         <f>MAX('[1]Tabelle 1'!F20:I20)</f>
         <v>84.14</v>
       </c>
-      <c r="F19" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J20=G19,"Cermine",IF('[1]Tabelle 1'!K20=G19,"Grobid",IF('[1]Tabelle 1'!L20=G19,"ParsCit",IF('[1]Tabelle 1'!M20=G19,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="I20" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <f>'[2]Tabelle 1'!F20</f>
+        <v>84.14</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J20=M20,"Cermine",IF('[1]Tabelle 1'!K20=M20,"Grobid",IF('[1]Tabelle 1'!L20=M20,"ParsCit",IF('[1]Tabelle 1'!M20=M20,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M20" s="2">
         <f>MAX('[1]Tabelle 1'!J20:M20)</f>
         <v>86.99</v>
       </c>
+      <c r="N20" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
+        <f>'[2]Tabelle 1'!G20</f>
+        <v>86.99</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="str">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="str">
         <f>'[1]Tabelle 1'!A21</f>
         <v>Section-References</v>
       </c>
-      <c r="B20" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B21=C20,"Cermine",IF('[1]Tabelle 1'!C21=C20,"Grobid",IF('[1]Tabelle 1'!D21=C20,"ParsCit",IF('[1]Tabelle 1'!E21=C20,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B21" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B21=C21,"Cermine",IF('[1]Tabelle 1'!C21=C21,"Grobid",IF('[1]Tabelle 1'!D21=C21,"ParsCit",IF('[1]Tabelle 1'!E21=C21,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C21" s="2">
         <f>MAX('[1]Tabelle 1'!B21:E21)</f>
         <v>62.71</v>
       </c>
-      <c r="D20" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F21=E20,"Cermine",IF('[1]Tabelle 1'!G21=E20,"Grobid",IF('[1]Tabelle 1'!H21=E20,"ParsCit",IF('[1]Tabelle 1'!I21=E20,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D21" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <f>'[2]Tabelle 1'!E21</f>
+        <v>63.03</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.32000000000000028</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F21=H21,"Cermine",IF('[1]Tabelle 1'!G21=H21,"Grobid",IF('[1]Tabelle 1'!H21=H21,"ParsCit",IF('[1]Tabelle 1'!I21=H21,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H21" s="2">
         <f>MAX('[1]Tabelle 1'!F21:I21)</f>
         <v>47.77</v>
       </c>
-      <c r="F20" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J21=G20,"Cermine",IF('[1]Tabelle 1'!K21=G20,"Grobid",IF('[1]Tabelle 1'!L21=G20,"ParsCit",IF('[1]Tabelle 1'!M21=G20,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="I21" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <f>'[2]Tabelle 1'!F21</f>
+        <v>48.11</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.33999999999999631</v>
+      </c>
+      <c r="L21" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J21=M21,"Cermine",IF('[1]Tabelle 1'!K21=M21,"Grobid",IF('[1]Tabelle 1'!L21=M21,"ParsCit",IF('[1]Tabelle 1'!M21=M21,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M21" s="2">
         <f>MAX('[1]Tabelle 1'!J21:M21)</f>
         <v>48.73</v>
       </c>
+      <c r="N21" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
+        <f>'[2]Tabelle 1'!G21</f>
+        <v>49.02</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="5"/>
+        <v>-0.29000000000000625</v>
+      </c>
+      <c r="Q21" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="str">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="str">
         <f>'[1]Tabelle 1'!A22</f>
         <v>References</v>
       </c>
-      <c r="B21" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B22=C21,"Cermine",IF('[1]Tabelle 1'!C22=C21,"Grobid",IF('[1]Tabelle 1'!D22=C21,"ParsCit",IF('[1]Tabelle 1'!E22=C21,"PDFX","none"))))</f>
+      <c r="B22" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B22=C22,"Cermine",IF('[1]Tabelle 1'!C22=C22,"Grobid",IF('[1]Tabelle 1'!D22=C22,"ParsCit",IF('[1]Tabelle 1'!E22=C22,"PDFX","none"))))</f>
         <v>ParsCit</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C22" s="2">
         <f>MAX('[1]Tabelle 1'!B22:E22)</f>
         <v>97.25</v>
       </c>
-      <c r="D21" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F22=E21,"Cermine",IF('[1]Tabelle 1'!G22=E21,"Grobid",IF('[1]Tabelle 1'!H22=E21,"ParsCit",IF('[1]Tabelle 1'!I22=E21,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D22" s="2" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <f>'[2]Tabelle 1'!E22</f>
+        <v>92.24</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0100000000000051</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F22=H22,"Cermine",IF('[1]Tabelle 1'!G22=H22,"Grobid",IF('[1]Tabelle 1'!H22=H22,"ParsCit",IF('[1]Tabelle 1'!I22=H22,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H22" s="2">
         <f>MAX('[1]Tabelle 1'!F22:I22)</f>
         <v>90.93</v>
       </c>
-      <c r="F21" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J22=G21,"Cermine",IF('[1]Tabelle 1'!K22=G21,"Grobid",IF('[1]Tabelle 1'!L22=G21,"ParsCit",IF('[1]Tabelle 1'!M22=G21,"PDFX","none"))))</f>
+      <c r="I22" s="2" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <f>'[2]Tabelle 1'!F22</f>
+        <v>91.57</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.63999999999998636</v>
+      </c>
+      <c r="L22" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J22=M22,"Cermine",IF('[1]Tabelle 1'!K22=M22,"Grobid",IF('[1]Tabelle 1'!L22=M22,"ParsCit",IF('[1]Tabelle 1'!M22=M22,"PDFX","none"))))</f>
         <v>ParsCit</v>
       </c>
-      <c r="G21" s="3">
+      <c r="M22" s="2">
         <f>MAX('[1]Tabelle 1'!J22:M22)</f>
         <v>92.44</v>
       </c>
+      <c r="N22" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <f>'[2]Tabelle 1'!G22</f>
+        <v>89.11</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3299999999999983</v>
+      </c>
+      <c r="Q22" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="str">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="str">
         <f>'[1]Tabelle 1'!A23</f>
         <v>Average</v>
       </c>
-      <c r="B23" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!B23=C23,"Cermine",IF('[1]Tabelle 1'!C23=C23,"Grobid",IF('[1]Tabelle 1'!D23=C23,"ParsCit",IF('[1]Tabelle 1'!E23=C23,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="B24" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!B23=C24,"Cermine",IF('[1]Tabelle 1'!C23=C24,"Grobid",IF('[1]Tabelle 1'!D23=C24,"ParsCit",IF('[1]Tabelle 1'!E23=C24,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="C24" s="2">
         <f>MAX('[1]Tabelle 1'!B23:E23)</f>
         <v>86.45</v>
       </c>
-      <c r="D23" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!F23=E23,"Cermine",IF('[1]Tabelle 1'!G23=E23,"Grobid",IF('[1]Tabelle 1'!H23=E23,"ParsCit",IF('[1]Tabelle 1'!I23=E23,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D24" s="2" t="b">
+        <f>B24="Grobid"</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <f>'[2]Tabelle 1'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <f>C24-E24</f>
+        <v>86.45</v>
+      </c>
+      <c r="G24" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!F23=H24,"Cermine",IF('[1]Tabelle 1'!G23=H24,"Grobid",IF('[1]Tabelle 1'!H23=H24,"ParsCit",IF('[1]Tabelle 1'!I23=H24,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="H24" s="2">
         <f>MAX('[1]Tabelle 1'!F23:I23)</f>
         <v>65.3</v>
       </c>
-      <c r="F23" s="3" t="str">
-        <f>IF('[1]Tabelle 1'!J23=G23,"Cermine",IF('[1]Tabelle 1'!K23=G23,"Grobid",IF('[1]Tabelle 1'!L23=G23,"ParsCit",IF('[1]Tabelle 1'!M23=G23,"PDFX","none"))))</f>
-        <v>Grobid</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="I24" s="2" t="b">
+        <f>G24="Grobid"</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <f>'[2]Tabelle 1'!F24</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <f>H24-J24</f>
+        <v>65.3</v>
+      </c>
+      <c r="L24" s="2" t="str">
+        <f>IF('[1]Tabelle 1'!J23=M24,"Cermine",IF('[1]Tabelle 1'!K23=M24,"Grobid",IF('[1]Tabelle 1'!L23=M24,"ParsCit",IF('[1]Tabelle 1'!M23=M24,"PDFX","none"))))</f>
+        <v>Grobid</v>
+      </c>
+      <c r="M24" s="2">
         <f>MAX('[1]Tabelle 1'!J23:M23)</f>
         <v>64.760000000000005</v>
       </c>
+      <c r="N24" s="2" t="b">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="2">
+        <f>'[2]Tabelle 1'!G24</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="5"/>
+        <v>64.760000000000005</v>
+      </c>
+      <c r="Q24" s="2" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G21 B23:G23">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>NOT(AND(EXACT($B2,$D2),EXACT($D2,$F2)))</formula>
+  <conditionalFormatting sqref="B3:F24">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$D3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:K24">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$I3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:Q24">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$N3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>